<commit_message>
nutrient and CPUE analysis
</commit_message>
<xml_diff>
--- a/FishLandings/output/statistics_v2.xlsx
+++ b/FishLandings/output/statistics_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C008ADA-590A-6B4C-A79C-34E12BEE2B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0242DBDC-D798-ED46-AE85-84E47392FA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-3080" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Per Trap Stats" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Profit sheet for R" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Supp Table 1 Methods'!$B$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Supp Table 1 Methods'!$A$2:$H$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Supp Table 1 Methods v2'!$A$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="106">
   <si>
     <t xml:space="preserve">t </t>
   </si>
@@ -2653,38 +2653,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AC47"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="28.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="2" customWidth="1"/>
-    <col min="4" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="24.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.6640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="16.6640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="16.6640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="28.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
+    <col min="3" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="24.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="22.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.6640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="16.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="53"/>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2693,160 +2693,156 @@
       <c r="F1" s="53"/>
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="71" t="s">
+      <c r="I1" s="71" t="s">
         <v>73</v>
       </c>
+      <c r="J1" s="71"/>
       <c r="K1" s="71"/>
       <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71" t="s">
+      <c r="M1" s="71" t="s">
         <v>84</v>
       </c>
+      <c r="N1" s="71"/>
       <c r="O1" s="71"/>
       <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71" t="s">
+      <c r="Q1" s="71" t="s">
         <v>85</v>
       </c>
+      <c r="R1" s="71"/>
       <c r="S1" s="71"/>
       <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71" t="s">
+      <c r="U1" s="71" t="s">
         <v>88</v>
       </c>
+      <c r="V1" s="71"/>
       <c r="W1" s="71"/>
       <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71" t="s">
+      <c r="Y1" s="71" t="s">
         <v>89</v>
       </c>
+      <c r="Z1" s="71"/>
       <c r="AA1" s="71"/>
       <c r="AB1" s="71"/>
-      <c r="AC1" s="71"/>
-    </row>
-    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="54" t="s">
         <v>33</v>
       </c>
+      <c r="C2" s="55" t="s">
+        <v>47</v>
+      </c>
       <c r="D2" s="55" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="J2" s="55" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" s="55" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M2" s="55" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N2" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="55" t="s">
+      <c r="R2" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="S2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="55" t="s">
+      <c r="T2" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="U2" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="Z2" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="T2" s="55" t="s">
+      <c r="AA2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="AB2" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="V2" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y2" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z2" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA2" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB2" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC2" s="55" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="57" t="s">
         <v>34</v>
       </c>
+      <c r="C3" s="58">
+        <v>54</v>
+      </c>
       <c r="D3" s="58">
-        <v>54</v>
+        <v>23.2</v>
       </c>
       <c r="E3" s="58">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="58">
         <v>25.2</v>
       </c>
-      <c r="G3" s="59">
+      <c r="F3" s="59">
         <v>4.2560000000000001E-2</v>
       </c>
-      <c r="H3" s="60">
+      <c r="G3" s="60">
         <v>2.8679999999999999</v>
       </c>
-      <c r="I3" s="61">
-        <v>250</v>
+      <c r="H3" s="61">
+        <v>250</v>
+      </c>
+      <c r="I3" s="56">
+        <v>100</v>
       </c>
       <c r="J3" s="56">
-        <v>100</v>
-      </c>
-      <c r="K3" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K3" s="61">
+        <v>100</v>
       </c>
       <c r="L3" s="61">
         <v>100</v>
@@ -2858,173 +2854,167 @@
         <v>100</v>
       </c>
       <c r="O3" s="61">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P3" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q3" s="61">
+        <v>170</v>
+      </c>
+      <c r="R3" s="61">
+        <v>200</v>
+      </c>
+      <c r="S3" s="61">
+        <v>170</v>
+      </c>
+      <c r="T3" s="61">
+        <v>200</v>
+      </c>
+      <c r="U3" s="61">
+        <v>150</v>
+      </c>
+      <c r="V3" s="61">
+        <v>200</v>
+      </c>
+      <c r="W3" s="61">
         <v>120</v>
       </c>
-      <c r="Q3" s="61">
-        <v>150</v>
-      </c>
-      <c r="R3" s="61">
-        <v>170</v>
-      </c>
-      <c r="S3" s="61">
-        <v>200</v>
-      </c>
-      <c r="T3" s="61">
-        <v>170</v>
-      </c>
-      <c r="U3" s="61">
-        <v>200</v>
-      </c>
-      <c r="V3" s="61">
-        <v>150</v>
-      </c>
-      <c r="W3" s="61">
-        <v>200</v>
-      </c>
       <c r="X3" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y3" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z3" s="61">
         <v>220</v>
       </c>
       <c r="AA3" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB3" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC3" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="53" t="s">
         <v>34</v>
       </c>
+      <c r="C4" s="58">
+        <v>21</v>
+      </c>
       <c r="D4" s="58">
-        <v>21</v>
+        <v>7.8</v>
       </c>
       <c r="E4" s="58">
-        <v>7.8</v>
-      </c>
-      <c r="F4" s="58">
         <v>7.1</v>
       </c>
+      <c r="F4" s="62">
+        <v>8.8999999999999999E-3</v>
+      </c>
       <c r="G4" s="62">
-        <v>8.8999999999999999E-3</v>
+        <v>3.278</v>
       </c>
       <c r="H4" s="62">
-        <v>3.278</v>
-      </c>
-      <c r="I4" s="62">
-        <v>250</v>
+        <v>250</v>
+      </c>
+      <c r="I4" s="56">
+        <v>100</v>
       </c>
       <c r="J4" s="56">
-        <v>100</v>
-      </c>
-      <c r="K4" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K4" s="62">
+        <v>100</v>
       </c>
       <c r="L4" s="62">
         <v>100</v>
       </c>
-      <c r="M4" s="62">
+      <c r="M4" s="61">
         <v>100</v>
       </c>
       <c r="N4" s="61">
         <v>100</v>
       </c>
-      <c r="O4" s="61">
-        <v>100</v>
+      <c r="O4" s="62">
+        <v>120</v>
       </c>
       <c r="P4" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q4" s="61">
+        <v>170</v>
+      </c>
+      <c r="R4" s="61">
+        <v>200</v>
+      </c>
+      <c r="S4" s="62">
+        <v>170</v>
+      </c>
+      <c r="T4" s="62">
+        <v>200</v>
+      </c>
+      <c r="U4" s="61">
+        <v>150</v>
+      </c>
+      <c r="V4" s="61">
+        <v>200</v>
+      </c>
+      <c r="W4" s="61">
         <v>120</v>
       </c>
-      <c r="Q4" s="62">
-        <v>150</v>
-      </c>
-      <c r="R4" s="61">
-        <v>170</v>
-      </c>
-      <c r="S4" s="61">
-        <v>200</v>
-      </c>
-      <c r="T4" s="62">
-        <v>170</v>
-      </c>
-      <c r="U4" s="62">
-        <v>200</v>
-      </c>
-      <c r="V4" s="61">
-        <v>150</v>
-      </c>
-      <c r="W4" s="61">
-        <v>200</v>
-      </c>
       <c r="X4" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y4" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z4" s="61">
         <v>220</v>
       </c>
       <c r="AA4" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB4" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC4" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="57" t="s">
+      <c r="B5" s="57" t="s">
         <v>34</v>
       </c>
+      <c r="C5" s="58">
+        <v>27</v>
+      </c>
       <c r="D5" s="58">
-        <v>27</v>
+        <v>12.3</v>
       </c>
       <c r="E5" s="58">
-        <v>12.3</v>
-      </c>
-      <c r="F5" s="58">
         <v>12.2</v>
       </c>
-      <c r="G5" s="59">
+      <c r="F5" s="59">
         <v>3.61E-2</v>
       </c>
-      <c r="H5" s="60">
+      <c r="G5" s="60">
         <v>3.13</v>
       </c>
-      <c r="I5" s="61">
-        <v>250</v>
+      <c r="H5" s="61">
+        <v>250</v>
+      </c>
+      <c r="I5" s="56">
+        <v>100</v>
       </c>
       <c r="J5" s="56">
-        <v>100</v>
-      </c>
-      <c r="K5" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K5" s="61">
+        <v>100</v>
       </c>
       <c r="L5" s="61">
         <v>100</v>
@@ -3036,84 +3026,81 @@
         <v>100</v>
       </c>
       <c r="O5" s="61">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P5" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q5" s="61">
+        <v>170</v>
+      </c>
+      <c r="R5" s="61">
+        <v>200</v>
+      </c>
+      <c r="S5" s="62">
+        <v>170</v>
+      </c>
+      <c r="T5" s="62">
+        <v>200</v>
+      </c>
+      <c r="U5" s="61">
+        <v>150</v>
+      </c>
+      <c r="V5" s="61">
+        <v>200</v>
+      </c>
+      <c r="W5" s="61">
         <v>120</v>
       </c>
-      <c r="Q5" s="61">
-        <v>150</v>
-      </c>
-      <c r="R5" s="61">
-        <v>170</v>
-      </c>
-      <c r="S5" s="61">
-        <v>200</v>
-      </c>
-      <c r="T5" s="62">
-        <v>170</v>
-      </c>
-      <c r="U5" s="62">
-        <v>200</v>
-      </c>
-      <c r="V5" s="61">
-        <v>150</v>
-      </c>
-      <c r="W5" s="61">
-        <v>200</v>
-      </c>
       <c r="X5" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y5" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z5" s="61">
         <v>220</v>
       </c>
       <c r="AA5" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB5" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC5" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="57" t="s">
+      <c r="B6" s="57" t="s">
         <v>34</v>
       </c>
+      <c r="C6" s="58">
+        <v>70</v>
+      </c>
       <c r="D6" s="58">
-        <v>70</v>
+        <v>35.5</v>
       </c>
       <c r="E6" s="58">
-        <v>35.5</v>
-      </c>
-      <c r="F6" s="58">
         <v>41.2</v>
       </c>
-      <c r="G6" s="59">
+      <c r="F6" s="59">
         <v>2.673E-2</v>
       </c>
-      <c r="H6" s="60">
+      <c r="G6" s="60">
         <v>2.984</v>
       </c>
-      <c r="I6" s="61">
-        <v>250</v>
+      <c r="H6" s="61">
+        <v>250</v>
+      </c>
+      <c r="I6" s="56">
+        <v>100</v>
       </c>
       <c r="J6" s="56">
-        <v>100</v>
-      </c>
-      <c r="K6" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K6" s="61">
+        <v>100</v>
       </c>
       <c r="L6" s="61">
         <v>100</v>
@@ -3125,84 +3112,81 @@
         <v>100</v>
       </c>
       <c r="O6" s="61">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P6" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q6" s="61">
+        <v>170</v>
+      </c>
+      <c r="R6" s="61">
+        <v>200</v>
+      </c>
+      <c r="S6" s="62">
+        <v>170</v>
+      </c>
+      <c r="T6" s="62">
+        <v>200</v>
+      </c>
+      <c r="U6" s="61">
+        <v>150</v>
+      </c>
+      <c r="V6" s="61">
+        <v>200</v>
+      </c>
+      <c r="W6" s="61">
         <v>120</v>
       </c>
-      <c r="Q6" s="61">
-        <v>150</v>
-      </c>
-      <c r="R6" s="61">
-        <v>170</v>
-      </c>
-      <c r="S6" s="61">
-        <v>200</v>
-      </c>
-      <c r="T6" s="62">
-        <v>170</v>
-      </c>
-      <c r="U6" s="62">
-        <v>200</v>
-      </c>
-      <c r="V6" s="61">
-        <v>150</v>
-      </c>
-      <c r="W6" s="61">
-        <v>200</v>
-      </c>
       <c r="X6" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y6" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z6" s="61">
         <v>220</v>
       </c>
       <c r="AA6" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB6" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC6" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="57" t="s">
+      <c r="B7" s="57" t="s">
         <v>34</v>
       </c>
+      <c r="C7" s="58">
+        <v>100</v>
+      </c>
       <c r="D7" s="58">
-        <v>100</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="E7" s="58">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="F7" s="58">
         <v>46.4</v>
       </c>
-      <c r="G7" s="59">
+      <c r="F7" s="59">
         <v>5.1029999999999999E-2</v>
       </c>
-      <c r="H7" s="60">
+      <c r="G7" s="60">
         <v>2.7149999999999999</v>
       </c>
-      <c r="I7" s="61">
-        <v>250</v>
+      <c r="H7" s="61">
+        <v>250</v>
+      </c>
+      <c r="I7" s="56">
+        <v>100</v>
       </c>
       <c r="J7" s="56">
-        <v>100</v>
-      </c>
-      <c r="K7" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K7" s="61">
+        <v>100</v>
       </c>
       <c r="L7" s="61">
         <v>100</v>
@@ -3214,84 +3198,81 @@
         <v>100</v>
       </c>
       <c r="O7" s="61">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P7" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q7" s="61">
+        <v>170</v>
+      </c>
+      <c r="R7" s="61">
+        <v>200</v>
+      </c>
+      <c r="S7" s="62">
+        <v>170</v>
+      </c>
+      <c r="T7" s="62">
+        <v>200</v>
+      </c>
+      <c r="U7" s="61">
+        <v>150</v>
+      </c>
+      <c r="V7" s="61">
+        <v>200</v>
+      </c>
+      <c r="W7" s="61">
         <v>120</v>
       </c>
-      <c r="Q7" s="61">
-        <v>150</v>
-      </c>
-      <c r="R7" s="61">
-        <v>170</v>
-      </c>
-      <c r="S7" s="61">
-        <v>200</v>
-      </c>
-      <c r="T7" s="62">
-        <v>170</v>
-      </c>
-      <c r="U7" s="62">
-        <v>200</v>
-      </c>
-      <c r="V7" s="61">
-        <v>150</v>
-      </c>
-      <c r="W7" s="61">
-        <v>200</v>
-      </c>
       <c r="X7" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y7" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z7" s="61">
         <v>220</v>
       </c>
       <c r="AA7" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB7" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC7" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="57" t="s">
+      <c r="B8" s="57" t="s">
         <v>34</v>
       </c>
+      <c r="C8" s="58">
+        <v>90</v>
+      </c>
       <c r="D8" s="58">
-        <v>90</v>
+        <v>48.8</v>
       </c>
       <c r="E8" s="58">
-        <v>48.8</v>
-      </c>
-      <c r="F8" s="58">
         <v>59.7</v>
       </c>
-      <c r="G8" s="59">
+      <c r="F8" s="59">
         <v>1.89E-2</v>
       </c>
-      <c r="H8" s="60">
+      <c r="G8" s="60">
         <v>2.99</v>
       </c>
-      <c r="I8" s="61">
-        <v>250</v>
+      <c r="H8" s="61">
+        <v>250</v>
+      </c>
+      <c r="I8" s="56">
+        <v>100</v>
       </c>
       <c r="J8" s="56">
-        <v>100</v>
-      </c>
-      <c r="K8" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K8" s="61">
+        <v>100</v>
       </c>
       <c r="L8" s="61">
         <v>100</v>
@@ -3303,268 +3284,259 @@
         <v>100</v>
       </c>
       <c r="O8" s="61">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P8" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q8" s="61">
+        <v>170</v>
+      </c>
+      <c r="R8" s="61">
+        <v>200</v>
+      </c>
+      <c r="S8" s="62">
+        <v>170</v>
+      </c>
+      <c r="T8" s="62">
+        <v>200</v>
+      </c>
+      <c r="U8" s="61">
+        <v>150</v>
+      </c>
+      <c r="V8" s="61">
+        <v>200</v>
+      </c>
+      <c r="W8" s="61">
         <v>120</v>
       </c>
-      <c r="Q8" s="61">
-        <v>150</v>
-      </c>
-      <c r="R8" s="61">
-        <v>170</v>
-      </c>
-      <c r="S8" s="61">
-        <v>200</v>
-      </c>
-      <c r="T8" s="62">
-        <v>170</v>
-      </c>
-      <c r="U8" s="62">
-        <v>200</v>
-      </c>
-      <c r="V8" s="61">
-        <v>150</v>
-      </c>
-      <c r="W8" s="61">
-        <v>200</v>
-      </c>
       <c r="X8" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y8" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z8" s="61">
         <v>220</v>
       </c>
       <c r="AA8" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB8" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC8" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="53" t="s">
         <v>66</v>
       </c>
+      <c r="C9" s="58">
+        <v>23</v>
+      </c>
       <c r="D9" s="58">
-        <v>23</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E9" s="58">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="F9" s="58">
         <v>9.1999999999999993</v>
       </c>
+      <c r="F9" s="62">
+        <v>3.1199999999999999E-2</v>
+      </c>
       <c r="G9" s="62">
-        <v>3.1199999999999999E-2</v>
+        <v>2.9529999999999998</v>
       </c>
       <c r="H9" s="62">
-        <v>2.9529999999999998</v>
-      </c>
-      <c r="I9" s="62">
         <v>0</v>
       </c>
+      <c r="I9" s="56">
+        <v>100</v>
+      </c>
       <c r="J9" s="56">
-        <v>100</v>
-      </c>
-      <c r="K9" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K9" s="62">
+        <v>100</v>
       </c>
       <c r="L9" s="62">
         <v>100</v>
       </c>
-      <c r="M9" s="62">
+      <c r="M9" s="61">
         <v>100</v>
       </c>
       <c r="N9" s="61">
         <v>100</v>
       </c>
-      <c r="O9" s="61">
-        <v>100</v>
+      <c r="O9" s="62">
+        <v>120</v>
       </c>
       <c r="P9" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q9" s="61">
+        <v>170</v>
+      </c>
+      <c r="R9" s="61">
+        <v>200</v>
+      </c>
+      <c r="S9" s="62">
+        <v>170</v>
+      </c>
+      <c r="T9" s="62">
+        <v>200</v>
+      </c>
+      <c r="U9" s="61">
+        <v>150</v>
+      </c>
+      <c r="V9" s="61">
+        <v>200</v>
+      </c>
+      <c r="W9" s="61">
         <v>120</v>
       </c>
-      <c r="Q9" s="62">
-        <v>150</v>
-      </c>
-      <c r="R9" s="61">
-        <v>170</v>
-      </c>
-      <c r="S9" s="61">
-        <v>200</v>
-      </c>
-      <c r="T9" s="62">
-        <v>170</v>
-      </c>
-      <c r="U9" s="62">
-        <v>200</v>
-      </c>
-      <c r="V9" s="61">
-        <v>150</v>
-      </c>
-      <c r="W9" s="61">
-        <v>200</v>
-      </c>
       <c r="X9" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y9" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z9" s="61">
         <v>220</v>
       </c>
       <c r="AA9" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB9" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC9" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="53" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="53" t="s">
         <v>66</v>
       </c>
+      <c r="C10" s="58">
+        <v>16</v>
+      </c>
       <c r="D10" s="58">
-        <v>16</v>
+        <v>10.6</v>
       </c>
       <c r="E10" s="58">
-        <v>10.6</v>
-      </c>
-      <c r="F10" s="58">
         <v>10.1</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>50</v>
       </c>
       <c r="G10" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="62">
+      <c r="H10" s="62">
         <v>0</v>
       </c>
+      <c r="I10" s="56">
+        <v>100</v>
+      </c>
       <c r="J10" s="56">
-        <v>100</v>
-      </c>
-      <c r="K10" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K10" s="62">
+        <v>100</v>
       </c>
       <c r="L10" s="62">
         <v>100</v>
       </c>
-      <c r="M10" s="62">
+      <c r="M10" s="61">
         <v>100</v>
       </c>
       <c r="N10" s="61">
         <v>100</v>
       </c>
-      <c r="O10" s="61">
-        <v>100</v>
+      <c r="O10" s="62">
+        <v>120</v>
       </c>
       <c r="P10" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q10" s="61">
+        <v>170</v>
+      </c>
+      <c r="R10" s="61">
+        <v>200</v>
+      </c>
+      <c r="S10" s="62">
+        <v>170</v>
+      </c>
+      <c r="T10" s="62">
+        <v>200</v>
+      </c>
+      <c r="U10" s="61">
+        <v>150</v>
+      </c>
+      <c r="V10" s="61">
+        <v>200</v>
+      </c>
+      <c r="W10" s="61">
         <v>120</v>
       </c>
-      <c r="Q10" s="62">
-        <v>150</v>
-      </c>
-      <c r="R10" s="61">
-        <v>170</v>
-      </c>
-      <c r="S10" s="61">
-        <v>200</v>
-      </c>
-      <c r="T10" s="62">
-        <v>170</v>
-      </c>
-      <c r="U10" s="62">
-        <v>200</v>
-      </c>
-      <c r="V10" s="61">
-        <v>150</v>
-      </c>
-      <c r="W10" s="61">
-        <v>200</v>
-      </c>
       <c r="X10" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y10" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z10" s="61">
         <v>220</v>
       </c>
       <c r="AA10" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB10" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC10" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="57" t="s">
         <v>42</v>
       </c>
+      <c r="C11" s="58">
+        <v>20.3</v>
+      </c>
       <c r="D11" s="58">
-        <v>20.3</v>
+        <v>13.5</v>
       </c>
       <c r="E11" s="58">
-        <v>13.5</v>
-      </c>
-      <c r="F11" s="58">
         <v>13.4</v>
       </c>
+      <c r="F11" s="60">
+        <v>1.26E-2</v>
+      </c>
       <c r="G11" s="60">
-        <v>1.26E-2</v>
-      </c>
-      <c r="H11" s="60">
         <v>3.04</v>
       </c>
-      <c r="I11" s="61">
-        <v>250</v>
+      <c r="H11" s="61">
+        <v>250</v>
+      </c>
+      <c r="I11" s="56">
+        <v>100</v>
       </c>
       <c r="J11" s="56">
-        <v>100</v>
-      </c>
-      <c r="K11" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K11" s="61">
+        <v>150</v>
       </c>
       <c r="L11" s="61">
         <v>150</v>
       </c>
       <c r="M11" s="61">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N11" s="61">
         <v>100</v>
@@ -3576,10 +3548,10 @@
         <v>100</v>
       </c>
       <c r="Q11" s="61">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="R11" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S11" s="61">
         <v>200</v>
@@ -3588,2474 +3560,2390 @@
         <v>200</v>
       </c>
       <c r="U11" s="61">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="V11" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W11" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="X11" s="61">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="Y11" s="61">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="Z11" s="61">
         <v>220</v>
       </c>
       <c r="AA11" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB11" s="61">
         <v>150</v>
       </c>
-      <c r="AC11" s="61">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="57" t="s">
+      <c r="B12" s="57" t="s">
         <v>36</v>
       </c>
+      <c r="C12" s="58">
+        <v>30</v>
+      </c>
       <c r="D12" s="58">
-        <v>30</v>
+        <v>18.5</v>
       </c>
       <c r="E12" s="58">
-        <v>18.5</v>
-      </c>
-      <c r="F12" s="58">
         <v>19.399999999999999</v>
       </c>
+      <c r="F12" s="60">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="G12" s="60">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H12" s="60">
         <v>2.96</v>
       </c>
-      <c r="I12" s="61">
-        <v>250</v>
+      <c r="H12" s="61">
+        <v>250</v>
+      </c>
+      <c r="I12" s="56">
+        <v>100</v>
       </c>
       <c r="J12" s="56">
-        <v>100</v>
-      </c>
-      <c r="K12" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K12" s="61">
+        <v>100</v>
       </c>
       <c r="L12" s="61">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M12" s="61">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N12" s="61">
         <v>100</v>
       </c>
       <c r="O12" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P12" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q12" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R12" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S12" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T12" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U12" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V12" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W12" s="61">
         <v>200</v>
       </c>
       <c r="X12" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Y12" s="61">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Z12" s="61">
         <v>220</v>
       </c>
       <c r="AA12" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB12" s="61">
         <v>300</v>
       </c>
-      <c r="AC12" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="57" t="s">
+      <c r="B13" s="57" t="s">
         <v>41</v>
       </c>
+      <c r="C13" s="58">
+        <v>60</v>
+      </c>
       <c r="D13" s="58">
-        <v>60</v>
+        <v>34.1</v>
       </c>
       <c r="E13" s="58">
-        <v>34.1</v>
-      </c>
-      <c r="F13" s="58">
         <v>39.4</v>
       </c>
+      <c r="F13" s="60">
+        <v>3.9800000000000002E-2</v>
+      </c>
       <c r="G13" s="60">
-        <v>3.9800000000000002E-2</v>
-      </c>
-      <c r="H13" s="60">
         <v>2.86</v>
       </c>
-      <c r="I13" s="62">
-        <v>300</v>
+      <c r="H13" s="62">
+        <v>300</v>
+      </c>
+      <c r="I13" s="56">
+        <v>100</v>
       </c>
       <c r="J13" s="56">
-        <v>100</v>
-      </c>
-      <c r="K13" s="56">
+        <v>180</v>
+      </c>
+      <c r="K13" s="62">
         <v>180</v>
       </c>
       <c r="L13" s="62">
-        <v>180</v>
-      </c>
-      <c r="M13" s="62">
-        <v>200</v>
+        <v>200</v>
+      </c>
+      <c r="M13" s="61">
+        <v>100</v>
       </c>
       <c r="N13" s="61">
         <v>100</v>
       </c>
-      <c r="O13" s="61">
-        <v>100</v>
+      <c r="O13" s="62">
+        <v>200</v>
       </c>
       <c r="P13" s="62">
-        <v>200</v>
-      </c>
-      <c r="Q13" s="62">
-        <v>250</v>
+        <v>250</v>
+      </c>
+      <c r="Q13" s="61">
+        <v>170</v>
       </c>
       <c r="R13" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S13" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T13" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U13" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V13" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W13" s="61">
         <v>200</v>
       </c>
       <c r="X13" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Y13" s="61">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Z13" s="61">
         <v>220</v>
       </c>
-      <c r="AA13" s="61">
-        <v>220</v>
+      <c r="AA13" s="62">
+        <v>150</v>
       </c>
       <c r="AB13" s="62">
-        <v>150</v>
-      </c>
-      <c r="AC13" s="62">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="57" t="s">
+      <c r="B14" s="57" t="s">
         <v>41</v>
       </c>
+      <c r="C14" s="58">
+        <v>50</v>
+      </c>
       <c r="D14" s="58">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E14" s="58">
-        <v>29</v>
-      </c>
-      <c r="F14" s="58">
         <v>32.700000000000003</v>
       </c>
+      <c r="F14" s="60">
+        <v>-1.3260000000000001</v>
+      </c>
       <c r="G14" s="60">
-        <v>-1.3260000000000001</v>
-      </c>
-      <c r="H14" s="60">
         <v>0.88</v>
       </c>
-      <c r="I14" s="61">
-        <v>300</v>
+      <c r="H14" s="61">
+        <v>300</v>
+      </c>
+      <c r="I14" s="56">
+        <v>100</v>
       </c>
       <c r="J14" s="56">
-        <v>100</v>
-      </c>
-      <c r="K14" s="56">
+        <v>180</v>
+      </c>
+      <c r="K14" s="62">
         <v>180</v>
       </c>
       <c r="L14" s="62">
-        <v>180</v>
-      </c>
-      <c r="M14" s="62">
-        <v>200</v>
+        <v>200</v>
+      </c>
+      <c r="M14" s="61">
+        <v>100</v>
       </c>
       <c r="N14" s="61">
         <v>100</v>
       </c>
       <c r="O14" s="61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P14" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q14" s="61">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="R14" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S14" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T14" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U14" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V14" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W14" s="61">
         <v>200</v>
       </c>
       <c r="X14" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Y14" s="61">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Z14" s="61">
         <v>220</v>
       </c>
-      <c r="AA14" s="61">
-        <v>220</v>
+      <c r="AA14" s="62">
+        <v>150</v>
       </c>
       <c r="AB14" s="62">
-        <v>150</v>
-      </c>
-      <c r="AC14" s="62">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="57" t="s">
+      <c r="B15" s="57" t="s">
         <v>41</v>
       </c>
+      <c r="C15" s="58">
+        <v>60</v>
+      </c>
       <c r="D15" s="58">
-        <v>60</v>
+        <v>34.1</v>
       </c>
       <c r="E15" s="58">
-        <v>34.1</v>
-      </c>
-      <c r="F15" s="58">
         <v>39.4</v>
       </c>
+      <c r="F15" s="60">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="G15" s="60">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="H15" s="60">
         <v>2.75</v>
       </c>
-      <c r="I15" s="61">
-        <v>300</v>
+      <c r="H15" s="61">
+        <v>300</v>
+      </c>
+      <c r="I15" s="56">
+        <v>100</v>
       </c>
       <c r="J15" s="56">
-        <v>100</v>
-      </c>
-      <c r="K15" s="56">
+        <v>180</v>
+      </c>
+      <c r="K15" s="62">
         <v>180</v>
       </c>
       <c r="L15" s="62">
-        <v>180</v>
-      </c>
-      <c r="M15" s="62">
-        <v>200</v>
+        <v>200</v>
+      </c>
+      <c r="M15" s="61">
+        <v>100</v>
       </c>
       <c r="N15" s="61">
         <v>100</v>
       </c>
       <c r="O15" s="61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P15" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q15" s="61">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="R15" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S15" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T15" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U15" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V15" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W15" s="61">
         <v>200</v>
       </c>
       <c r="X15" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Y15" s="61">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Z15" s="61">
         <v>220</v>
       </c>
-      <c r="AA15" s="61">
-        <v>220</v>
+      <c r="AA15" s="62">
+        <v>150</v>
       </c>
       <c r="AB15" s="62">
-        <v>150</v>
-      </c>
-      <c r="AC15" s="62">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="57" t="s">
+      <c r="B16" s="57" t="s">
         <v>41</v>
       </c>
+      <c r="C16" s="58">
+        <v>72</v>
+      </c>
       <c r="D16" s="58">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E16" s="58">
-        <v>40</v>
-      </c>
-      <c r="F16" s="58">
         <v>47.4</v>
       </c>
+      <c r="F16" s="60">
+        <v>-0.78100000000000003</v>
+      </c>
       <c r="G16" s="60">
-        <v>-0.78100000000000003</v>
-      </c>
-      <c r="H16" s="60">
         <v>0.85</v>
       </c>
-      <c r="I16" s="61">
-        <v>300</v>
+      <c r="H16" s="61">
+        <v>300</v>
+      </c>
+      <c r="I16" s="56">
+        <v>100</v>
       </c>
       <c r="J16" s="56">
-        <v>100</v>
-      </c>
-      <c r="K16" s="56">
+        <v>180</v>
+      </c>
+      <c r="K16" s="62">
         <v>180</v>
       </c>
       <c r="L16" s="62">
-        <v>180</v>
-      </c>
-      <c r="M16" s="62">
-        <v>200</v>
+        <v>200</v>
+      </c>
+      <c r="M16" s="61">
+        <v>100</v>
       </c>
       <c r="N16" s="61">
         <v>100</v>
       </c>
       <c r="O16" s="61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P16" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q16" s="61">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="R16" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S16" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T16" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U16" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V16" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W16" s="61">
         <v>200</v>
       </c>
       <c r="X16" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Y16" s="61">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="Z16" s="61">
         <v>220</v>
       </c>
-      <c r="AA16" s="61">
-        <v>220</v>
+      <c r="AA16" s="62">
+        <v>150</v>
       </c>
       <c r="AB16" s="62">
-        <v>150</v>
-      </c>
-      <c r="AC16" s="62">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="57" t="s">
+      <c r="B17" s="57" t="s">
         <v>38</v>
       </c>
+      <c r="C17" s="58">
+        <v>76</v>
+      </c>
       <c r="D17" s="58">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="E17" s="58">
-        <v>42</v>
-      </c>
-      <c r="F17" s="58">
         <v>50.2</v>
       </c>
+      <c r="F17" s="60">
+        <v>0</v>
+      </c>
       <c r="G17" s="60">
-        <v>0</v>
-      </c>
-      <c r="H17" s="60">
         <v>1.0840000000000001</v>
       </c>
-      <c r="I17" s="61">
+      <c r="H17" s="61">
         <v>350</v>
       </c>
+      <c r="I17" s="56">
+        <v>100</v>
+      </c>
       <c r="J17" s="56">
-        <v>100</v>
-      </c>
-      <c r="K17" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K17" s="61">
+        <v>200</v>
       </c>
       <c r="L17" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M17" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N17" s="61">
         <v>100</v>
       </c>
       <c r="O17" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P17" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q17" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R17" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S17" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T17" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U17" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V17" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W17" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X17" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y17" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z17" s="61">
         <v>220</v>
       </c>
       <c r="AA17" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB17" s="61">
         <v>300</v>
       </c>
-      <c r="AC17" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="57" t="s">
+      <c r="B18" s="57" t="s">
         <v>38</v>
       </c>
+      <c r="C18" s="58">
+        <v>50</v>
+      </c>
       <c r="D18" s="58">
-        <v>50</v>
+        <v>23.6</v>
       </c>
       <c r="E18" s="58">
-        <v>23.6</v>
-      </c>
-      <c r="F18" s="58">
         <v>25.8</v>
       </c>
+      <c r="F18" s="60">
+        <v>1.7010000000000001E-2</v>
+      </c>
       <c r="G18" s="60">
-        <v>1.7010000000000001E-2</v>
-      </c>
-      <c r="H18" s="60">
         <v>3.0419999999999998</v>
       </c>
-      <c r="I18" s="61">
+      <c r="H18" s="61">
         <v>350</v>
       </c>
+      <c r="I18" s="56">
+        <v>100</v>
+      </c>
       <c r="J18" s="56">
-        <v>100</v>
-      </c>
-      <c r="K18" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K18" s="61">
+        <v>200</v>
       </c>
       <c r="L18" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M18" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N18" s="61">
         <v>100</v>
       </c>
       <c r="O18" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P18" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q18" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R18" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S18" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T18" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U18" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V18" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W18" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X18" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y18" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z18" s="61">
         <v>220</v>
       </c>
       <c r="AA18" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB18" s="61">
         <v>300</v>
       </c>
-      <c r="AC18" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="57" t="s">
+      <c r="B19" s="57" t="s">
         <v>38</v>
       </c>
+      <c r="C19" s="58">
+        <v>65</v>
+      </c>
       <c r="D19" s="58">
-        <v>65</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="E19" s="58">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="F19" s="58">
         <v>40.9</v>
       </c>
+      <c r="F19" s="60">
+        <v>1.6E-2</v>
+      </c>
       <c r="G19" s="60">
-        <v>1.6E-2</v>
-      </c>
-      <c r="H19" s="60">
         <v>3.077</v>
       </c>
-      <c r="I19" s="62">
+      <c r="H19" s="62">
         <v>350</v>
       </c>
+      <c r="I19" s="56">
+        <v>100</v>
+      </c>
       <c r="J19" s="56">
-        <v>100</v>
-      </c>
-      <c r="K19" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K19" s="61">
+        <v>200</v>
       </c>
       <c r="L19" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M19" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N19" s="61">
         <v>100</v>
       </c>
-      <c r="O19" s="61">
-        <v>100</v>
+      <c r="O19" s="62">
+        <v>230</v>
       </c>
       <c r="P19" s="62">
-        <v>230</v>
-      </c>
-      <c r="Q19" s="62">
         <v>270</v>
       </c>
+      <c r="Q19" s="61">
+        <v>170</v>
+      </c>
       <c r="R19" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S19" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T19" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U19" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V19" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W19" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X19" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y19" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z19" s="61">
         <v>220</v>
       </c>
       <c r="AA19" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB19" s="61">
         <v>300</v>
       </c>
-      <c r="AC19" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="57" t="s">
+      <c r="B20" s="57" t="s">
         <v>38</v>
       </c>
+      <c r="C20" s="58">
+        <v>87</v>
+      </c>
       <c r="D20" s="58">
-        <v>87</v>
+        <v>37.4</v>
       </c>
       <c r="E20" s="58">
-        <v>37.4</v>
-      </c>
-      <c r="F20" s="58">
         <v>43.9</v>
       </c>
+      <c r="F20" s="60">
+        <v>1.8710000000000001E-2</v>
+      </c>
       <c r="G20" s="60">
-        <v>1.8710000000000001E-2</v>
-      </c>
-      <c r="H20" s="60">
         <v>2.996</v>
       </c>
-      <c r="I20" s="61">
+      <c r="H20" s="61">
         <v>350</v>
       </c>
+      <c r="I20" s="56">
+        <v>100</v>
+      </c>
       <c r="J20" s="56">
-        <v>100</v>
-      </c>
-      <c r="K20" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K20" s="61">
+        <v>200</v>
       </c>
       <c r="L20" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M20" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N20" s="61">
         <v>100</v>
       </c>
       <c r="O20" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P20" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q20" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R20" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S20" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T20" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U20" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V20" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W20" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X20" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y20" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z20" s="61">
         <v>220</v>
       </c>
       <c r="AA20" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB20" s="61">
         <v>300</v>
       </c>
-      <c r="AC20" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="57" t="s">
+      <c r="B21" s="57" t="s">
         <v>38</v>
       </c>
+      <c r="C21" s="58">
+        <v>60</v>
+      </c>
       <c r="D21" s="58">
-        <v>60</v>
+        <v>34.1</v>
       </c>
       <c r="E21" s="58">
-        <v>34.1</v>
-      </c>
-      <c r="F21" s="58">
         <v>39.4</v>
       </c>
+      <c r="F21" s="60">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="G21" s="60">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H21" s="60">
         <v>2.84</v>
       </c>
-      <c r="I21" s="61">
+      <c r="H21" s="61">
         <v>350</v>
       </c>
+      <c r="I21" s="56">
+        <v>100</v>
+      </c>
       <c r="J21" s="56">
-        <v>100</v>
-      </c>
-      <c r="K21" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K21" s="61">
+        <v>200</v>
       </c>
       <c r="L21" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M21" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N21" s="61">
         <v>100</v>
       </c>
       <c r="O21" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P21" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q21" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R21" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S21" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T21" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U21" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V21" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W21" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X21" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y21" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z21" s="61">
         <v>220</v>
       </c>
       <c r="AA21" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB21" s="61">
         <v>300</v>
       </c>
-      <c r="AC21" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="57" t="s">
+      <c r="B22" s="57" t="s">
         <v>39</v>
       </c>
+      <c r="C22" s="58">
+        <v>35</v>
+      </c>
       <c r="D22" s="58">
-        <v>35</v>
+        <v>13.6</v>
       </c>
       <c r="E22" s="58">
-        <v>13.6</v>
-      </c>
-      <c r="F22" s="58">
         <v>14</v>
       </c>
+      <c r="F22" s="60">
+        <v>2.0480000000000002E-2</v>
+      </c>
       <c r="G22" s="60">
-        <v>2.0480000000000002E-2</v>
-      </c>
-      <c r="H22" s="60">
         <v>2.96</v>
       </c>
-      <c r="I22" s="61">
+      <c r="H22" s="61">
         <v>350</v>
       </c>
+      <c r="I22" s="56">
+        <v>100</v>
+      </c>
       <c r="J22" s="56">
-        <v>100</v>
-      </c>
-      <c r="K22" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K22" s="61">
+        <v>200</v>
       </c>
       <c r="L22" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M22" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N22" s="61">
         <v>100</v>
       </c>
       <c r="O22" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P22" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q22" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R22" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S22" s="61">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="T22" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="U22" s="61">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="V22" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W22" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X22" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y22" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z22" s="61">
         <v>220</v>
       </c>
       <c r="AA22" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB22" s="61">
         <v>300</v>
       </c>
-      <c r="AC22" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="53" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="53" t="s">
         <v>65</v>
       </c>
+      <c r="C23" s="58">
+        <v>19.3</v>
+      </c>
       <c r="D23" s="58">
-        <v>19.3</v>
+        <v>12.5</v>
       </c>
       <c r="E23" s="58">
-        <v>12.5</v>
-      </c>
-      <c r="F23" s="58">
         <v>12.3</v>
+      </c>
+      <c r="F23" s="62" t="s">
+        <v>50</v>
       </c>
       <c r="G23" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="62">
+      <c r="H23" s="62">
         <v>0</v>
       </c>
+      <c r="I23" s="56">
+        <v>100</v>
+      </c>
       <c r="J23" s="56">
-        <v>100</v>
-      </c>
-      <c r="K23" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K23" s="62">
+        <v>100</v>
       </c>
       <c r="L23" s="62">
         <v>100</v>
       </c>
-      <c r="M23" s="62">
+      <c r="M23" s="61">
         <v>100</v>
       </c>
       <c r="N23" s="61">
         <v>100</v>
       </c>
-      <c r="O23" s="61">
-        <v>100</v>
+      <c r="O23" s="62">
+        <v>120</v>
       </c>
       <c r="P23" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q23" s="61">
+        <v>170</v>
+      </c>
+      <c r="R23" s="61">
+        <v>200</v>
+      </c>
+      <c r="S23" s="62">
+        <v>170</v>
+      </c>
+      <c r="T23" s="62">
+        <v>200</v>
+      </c>
+      <c r="U23" s="61">
+        <v>150</v>
+      </c>
+      <c r="V23" s="61">
+        <v>200</v>
+      </c>
+      <c r="W23" s="62">
         <v>120</v>
       </c>
-      <c r="Q23" s="62">
-        <v>150</v>
-      </c>
-      <c r="R23" s="61">
-        <v>170</v>
-      </c>
-      <c r="S23" s="61">
-        <v>200</v>
-      </c>
-      <c r="T23" s="62">
-        <v>170</v>
-      </c>
-      <c r="U23" s="62">
-        <v>200</v>
-      </c>
-      <c r="V23" s="61">
-        <v>150</v>
-      </c>
-      <c r="W23" s="61">
-        <v>200</v>
-      </c>
       <c r="X23" s="62">
-        <v>120</v>
-      </c>
-      <c r="Y23" s="62">
-        <v>150</v>
+        <v>150</v>
+      </c>
+      <c r="Y23" s="61">
+        <v>220</v>
       </c>
       <c r="Z23" s="61">
         <v>220</v>
       </c>
-      <c r="AA23" s="61">
-        <v>220</v>
+      <c r="AA23" s="62">
+        <v>150</v>
       </c>
       <c r="AB23" s="62">
-        <v>150</v>
-      </c>
-      <c r="AC23" s="62">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="57" t="s">
+      <c r="B24" s="57" t="s">
         <v>40</v>
       </c>
+      <c r="C24" s="58">
+        <v>43</v>
+      </c>
       <c r="D24" s="58">
-        <v>43</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E24" s="58">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F24" s="58">
         <v>21</v>
       </c>
+      <c r="F24" s="60">
+        <v>1.38E-2</v>
+      </c>
       <c r="G24" s="60">
-        <v>1.38E-2</v>
-      </c>
-      <c r="H24" s="60">
         <v>3.05</v>
       </c>
-      <c r="I24" s="61">
-        <v>300</v>
+      <c r="H24" s="61">
+        <v>300</v>
+      </c>
+      <c r="I24" s="56">
+        <v>100</v>
       </c>
       <c r="J24" s="56">
-        <v>100</v>
-      </c>
-      <c r="K24" s="56">
+        <v>180</v>
+      </c>
+      <c r="K24" s="61">
         <v>180</v>
       </c>
       <c r="L24" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M24" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N24" s="61">
         <v>100</v>
       </c>
       <c r="O24" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P24" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q24" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R24" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S24" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T24" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U24" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V24" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W24" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X24" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y24" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z24" s="61">
         <v>220</v>
       </c>
       <c r="AA24" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB24" s="61">
         <v>300</v>
       </c>
-      <c r="AC24" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="57" t="s">
+      <c r="B25" s="57" t="s">
         <v>40</v>
       </c>
+      <c r="C25" s="58">
+        <v>36</v>
+      </c>
       <c r="D25" s="58">
-        <v>36</v>
+        <v>17.5</v>
       </c>
       <c r="E25" s="58">
-        <v>17.5</v>
-      </c>
-      <c r="F25" s="58">
         <v>18.2</v>
       </c>
+      <c r="F25" s="60">
+        <v>1.6899999999999998E-2</v>
+      </c>
       <c r="G25" s="60">
-        <v>1.6899999999999998E-2</v>
-      </c>
-      <c r="H25" s="60">
         <v>3.0779999999999998</v>
       </c>
-      <c r="I25" s="61">
-        <v>300</v>
+      <c r="H25" s="61">
+        <v>300</v>
+      </c>
+      <c r="I25" s="56">
+        <v>100</v>
       </c>
       <c r="J25" s="56">
-        <v>100</v>
-      </c>
-      <c r="K25" s="56">
+        <v>180</v>
+      </c>
+      <c r="K25" s="61">
         <v>180</v>
       </c>
       <c r="L25" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M25" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N25" s="61">
         <v>100</v>
       </c>
       <c r="O25" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P25" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q25" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R25" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S25" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T25" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U25" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V25" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W25" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X25" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y25" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z25" s="61">
         <v>220</v>
       </c>
       <c r="AA25" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB25" s="61">
         <v>300</v>
       </c>
-      <c r="AC25" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="57" t="s">
+      <c r="B26" s="57" t="s">
         <v>40</v>
       </c>
+      <c r="C26" s="58">
+        <v>45</v>
+      </c>
       <c r="D26" s="58">
-        <v>45</v>
+        <v>26.5</v>
       </c>
       <c r="E26" s="58">
-        <v>26.5</v>
-      </c>
-      <c r="F26" s="58">
         <v>29.3</v>
       </c>
+      <c r="F26" s="60">
+        <v>1.7999999999999999E-2</v>
+      </c>
       <c r="G26" s="60">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="H26" s="60">
         <v>2.92</v>
       </c>
-      <c r="I26" s="62">
-        <v>300</v>
+      <c r="H26" s="62">
+        <v>300</v>
+      </c>
+      <c r="I26" s="56">
+        <v>100</v>
       </c>
       <c r="J26" s="56">
-        <v>100</v>
-      </c>
-      <c r="K26" s="56">
+        <v>180</v>
+      </c>
+      <c r="K26" s="61">
         <v>180</v>
       </c>
       <c r="L26" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M26" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N26" s="61">
         <v>100</v>
       </c>
-      <c r="O26" s="61">
-        <v>100</v>
+      <c r="O26" s="62">
+        <v>230</v>
       </c>
       <c r="P26" s="62">
-        <v>230</v>
-      </c>
-      <c r="Q26" s="62">
         <v>270</v>
       </c>
+      <c r="Q26" s="61">
+        <v>170</v>
+      </c>
       <c r="R26" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S26" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T26" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U26" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V26" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W26" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X26" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y26" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z26" s="61">
         <v>220</v>
       </c>
       <c r="AA26" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB26" s="61">
         <v>300</v>
       </c>
-      <c r="AC26" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="57" t="s">
+      <c r="B27" s="57" t="s">
         <v>40</v>
       </c>
+      <c r="C27" s="58">
+        <v>40</v>
+      </c>
       <c r="D27" s="58">
-        <v>40</v>
+        <v>23.8</v>
       </c>
       <c r="E27" s="58">
-        <v>23.8</v>
-      </c>
-      <c r="F27" s="58">
         <v>26</v>
       </c>
+      <c r="F27" s="60">
+        <v>5.4599999999999996E-3</v>
+      </c>
       <c r="G27" s="60">
-        <v>5.4599999999999996E-3</v>
-      </c>
-      <c r="H27" s="60">
         <v>3.2970000000000002</v>
       </c>
-      <c r="I27" s="61">
-        <v>300</v>
+      <c r="H27" s="61">
+        <v>300</v>
+      </c>
+      <c r="I27" s="56">
+        <v>100</v>
       </c>
       <c r="J27" s="56">
-        <v>100</v>
-      </c>
-      <c r="K27" s="56">
+        <v>180</v>
+      </c>
+      <c r="K27" s="61">
         <v>180</v>
       </c>
       <c r="L27" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M27" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N27" s="61">
         <v>100</v>
       </c>
       <c r="O27" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P27" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q27" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R27" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S27" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T27" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U27" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V27" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W27" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="X27" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Y27" s="61">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="Z27" s="61">
         <v>220</v>
       </c>
       <c r="AA27" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB27" s="61">
         <v>300</v>
       </c>
-      <c r="AC27" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="57" t="s">
+      <c r="B28" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C28" s="58">
+        <v>75</v>
+      </c>
       <c r="D28" s="58">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E28" s="58">
-        <v>30</v>
-      </c>
-      <c r="F28" s="58">
         <v>34</v>
       </c>
+      <c r="F28" s="60">
+        <v>2.1000000000000001E-2</v>
+      </c>
       <c r="G28" s="60">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="H28" s="60">
         <v>2.91</v>
       </c>
-      <c r="I28" s="61">
-        <v>250</v>
+      <c r="H28" s="61">
+        <v>250</v>
+      </c>
+      <c r="I28" s="56">
+        <v>100</v>
       </c>
       <c r="J28" s="56">
-        <v>100</v>
-      </c>
-      <c r="K28" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K28" s="61">
+        <v>120</v>
       </c>
       <c r="L28" s="61">
+        <v>150</v>
+      </c>
+      <c r="M28" s="61">
+        <v>100</v>
+      </c>
+      <c r="N28" s="61">
+        <v>100</v>
+      </c>
+      <c r="O28" s="61">
         <v>120</v>
       </c>
-      <c r="M28" s="61">
-        <v>150</v>
-      </c>
-      <c r="N28" s="61">
-        <v>100</v>
-      </c>
-      <c r="O28" s="61">
-        <v>100</v>
-      </c>
       <c r="P28" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q28" s="61">
+        <v>170</v>
+      </c>
+      <c r="R28" s="61">
+        <v>200</v>
+      </c>
+      <c r="S28" s="61">
+        <v>170</v>
+      </c>
+      <c r="T28" s="61">
+        <v>200</v>
+      </c>
+      <c r="U28" s="61">
+        <v>150</v>
+      </c>
+      <c r="V28" s="61">
+        <v>200</v>
+      </c>
+      <c r="W28" s="61">
         <v>120</v>
       </c>
-      <c r="Q28" s="61">
-        <v>150</v>
-      </c>
-      <c r="R28" s="61">
-        <v>170</v>
-      </c>
-      <c r="S28" s="61">
-        <v>200</v>
-      </c>
-      <c r="T28" s="61">
-        <v>170</v>
-      </c>
-      <c r="U28" s="61">
-        <v>200</v>
-      </c>
-      <c r="V28" s="61">
-        <v>150</v>
-      </c>
-      <c r="W28" s="61">
-        <v>200</v>
-      </c>
       <c r="X28" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y28" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z28" s="61">
         <v>220</v>
       </c>
       <c r="AA28" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB28" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC28" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="57" t="s">
+      <c r="B29" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C29" s="58">
+        <v>35.200000000000003</v>
+      </c>
       <c r="D29" s="58">
-        <v>35.200000000000003</v>
+        <v>21.3</v>
       </c>
       <c r="E29" s="58">
-        <v>21.3</v>
-      </c>
-      <c r="F29" s="58">
         <v>22.8</v>
       </c>
+      <c r="F29" s="60">
+        <v>1.84E-2</v>
+      </c>
       <c r="G29" s="60">
-        <v>1.84E-2</v>
-      </c>
-      <c r="H29" s="60">
         <v>2.94</v>
       </c>
-      <c r="I29" s="61">
-        <v>250</v>
+      <c r="H29" s="61">
+        <v>250</v>
+      </c>
+      <c r="I29" s="56">
+        <v>100</v>
       </c>
       <c r="J29" s="56">
-        <v>100</v>
-      </c>
-      <c r="K29" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K29" s="61">
+        <v>120</v>
       </c>
       <c r="L29" s="61">
+        <v>150</v>
+      </c>
+      <c r="M29" s="61">
+        <v>100</v>
+      </c>
+      <c r="N29" s="61">
+        <v>100</v>
+      </c>
+      <c r="O29" s="61">
         <v>120</v>
       </c>
-      <c r="M29" s="61">
-        <v>150</v>
-      </c>
-      <c r="N29" s="61">
-        <v>100</v>
-      </c>
-      <c r="O29" s="61">
-        <v>100</v>
-      </c>
       <c r="P29" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q29" s="61">
+        <v>170</v>
+      </c>
+      <c r="R29" s="61">
+        <v>200</v>
+      </c>
+      <c r="S29" s="61">
+        <v>170</v>
+      </c>
+      <c r="T29" s="61">
+        <v>200</v>
+      </c>
+      <c r="U29" s="61">
+        <v>150</v>
+      </c>
+      <c r="V29" s="61">
+        <v>200</v>
+      </c>
+      <c r="W29" s="61">
         <v>120</v>
       </c>
-      <c r="Q29" s="61">
-        <v>150</v>
-      </c>
-      <c r="R29" s="61">
-        <v>170</v>
-      </c>
-      <c r="S29" s="61">
-        <v>200</v>
-      </c>
-      <c r="T29" s="61">
-        <v>170</v>
-      </c>
-      <c r="U29" s="61">
-        <v>200</v>
-      </c>
-      <c r="V29" s="61">
-        <v>150</v>
-      </c>
-      <c r="W29" s="61">
-        <v>200</v>
-      </c>
       <c r="X29" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y29" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z29" s="61">
         <v>220</v>
       </c>
       <c r="AA29" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB29" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC29" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="57" t="s">
+      <c r="B30" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C30" s="58">
+        <v>75</v>
+      </c>
       <c r="D30" s="58">
-        <v>75</v>
+        <v>41.5</v>
       </c>
       <c r="E30" s="58">
-        <v>41.5</v>
-      </c>
-      <c r="F30" s="58">
         <v>49.5</v>
       </c>
+      <c r="F30" s="60">
+        <v>1.6500000000000001E-2</v>
+      </c>
       <c r="G30" s="60">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="H30" s="60">
         <v>3.0409999999999999</v>
       </c>
-      <c r="I30" s="61">
-        <v>250</v>
+      <c r="H30" s="61">
+        <v>250</v>
+      </c>
+      <c r="I30" s="56">
+        <v>100</v>
       </c>
       <c r="J30" s="56">
-        <v>100</v>
-      </c>
-      <c r="K30" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K30" s="61">
+        <v>120</v>
       </c>
       <c r="L30" s="61">
+        <v>150</v>
+      </c>
+      <c r="M30" s="61">
+        <v>100</v>
+      </c>
+      <c r="N30" s="61">
+        <v>100</v>
+      </c>
+      <c r="O30" s="61">
+        <v>200</v>
+      </c>
+      <c r="P30" s="61">
+        <v>250</v>
+      </c>
+      <c r="Q30" s="61">
+        <v>170</v>
+      </c>
+      <c r="R30" s="61">
+        <v>200</v>
+      </c>
+      <c r="S30" s="61">
+        <v>170</v>
+      </c>
+      <c r="T30" s="61">
+        <v>200</v>
+      </c>
+      <c r="U30" s="61">
+        <v>150</v>
+      </c>
+      <c r="V30" s="61">
+        <v>200</v>
+      </c>
+      <c r="W30" s="61">
         <v>120</v>
       </c>
-      <c r="M30" s="61">
-        <v>150</v>
-      </c>
-      <c r="N30" s="61">
-        <v>100</v>
-      </c>
-      <c r="O30" s="61">
-        <v>100</v>
-      </c>
-      <c r="P30" s="61">
-        <v>200</v>
-      </c>
-      <c r="Q30" s="61">
-        <v>250</v>
-      </c>
-      <c r="R30" s="61">
-        <v>170</v>
-      </c>
-      <c r="S30" s="61">
-        <v>200</v>
-      </c>
-      <c r="T30" s="61">
-        <v>170</v>
-      </c>
-      <c r="U30" s="61">
-        <v>200</v>
-      </c>
-      <c r="V30" s="61">
-        <v>150</v>
-      </c>
-      <c r="W30" s="61">
-        <v>200</v>
-      </c>
       <c r="X30" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y30" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z30" s="61">
         <v>220</v>
       </c>
       <c r="AA30" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB30" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC30" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="57" t="s">
+      <c r="B31" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C31" s="58">
+        <v>34</v>
+      </c>
       <c r="D31" s="58">
-        <v>34</v>
+        <v>15.8</v>
       </c>
       <c r="E31" s="58">
-        <v>15.8</v>
-      </c>
-      <c r="F31" s="58">
         <v>16.2</v>
       </c>
+      <c r="F31" s="60">
+        <v>1.41E-2</v>
+      </c>
       <c r="G31" s="60">
-        <v>1.41E-2</v>
-      </c>
-      <c r="H31" s="60">
         <v>3.14</v>
       </c>
-      <c r="I31" s="62">
-        <v>250</v>
+      <c r="H31" s="62">
+        <v>250</v>
+      </c>
+      <c r="I31" s="56">
+        <v>100</v>
       </c>
       <c r="J31" s="56">
-        <v>100</v>
-      </c>
-      <c r="K31" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K31" s="62">
+        <v>120</v>
       </c>
       <c r="L31" s="62">
+        <v>150</v>
+      </c>
+      <c r="M31" s="61">
+        <v>100</v>
+      </c>
+      <c r="N31" s="61">
+        <v>100</v>
+      </c>
+      <c r="O31" s="62">
         <v>120</v>
       </c>
-      <c r="M31" s="62">
-        <v>150</v>
-      </c>
-      <c r="N31" s="61">
-        <v>100</v>
-      </c>
-      <c r="O31" s="61">
-        <v>100</v>
-      </c>
       <c r="P31" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q31" s="61">
+        <v>170</v>
+      </c>
+      <c r="R31" s="61">
+        <v>200</v>
+      </c>
+      <c r="S31" s="61">
+        <v>170</v>
+      </c>
+      <c r="T31" s="61">
+        <v>200</v>
+      </c>
+      <c r="U31" s="61">
+        <v>150</v>
+      </c>
+      <c r="V31" s="61">
+        <v>200</v>
+      </c>
+      <c r="W31" s="61">
         <v>120</v>
       </c>
-      <c r="Q31" s="62">
-        <v>150</v>
-      </c>
-      <c r="R31" s="61">
-        <v>170</v>
-      </c>
-      <c r="S31" s="61">
-        <v>200</v>
-      </c>
-      <c r="T31" s="61">
-        <v>170</v>
-      </c>
-      <c r="U31" s="61">
-        <v>200</v>
-      </c>
-      <c r="V31" s="61">
-        <v>150</v>
-      </c>
-      <c r="W31" s="61">
-        <v>200</v>
-      </c>
       <c r="X31" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y31" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z31" s="61">
         <v>220</v>
       </c>
       <c r="AA31" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB31" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC31" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="57" t="s">
+      <c r="B32" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C32" s="58">
+        <v>70</v>
+      </c>
       <c r="D32" s="58">
-        <v>70</v>
+        <v>26.3</v>
       </c>
       <c r="E32" s="58">
-        <v>26.3</v>
-      </c>
-      <c r="F32" s="58">
         <v>29.2</v>
       </c>
+      <c r="F32" s="60">
+        <v>1.15E-2</v>
+      </c>
       <c r="G32" s="60">
-        <v>1.15E-2</v>
-      </c>
-      <c r="H32" s="60">
         <v>3.18</v>
       </c>
-      <c r="I32" s="61">
-        <v>250</v>
+      <c r="H32" s="61">
+        <v>250</v>
+      </c>
+      <c r="I32" s="56">
+        <v>100</v>
       </c>
       <c r="J32" s="56">
-        <v>100</v>
-      </c>
-      <c r="K32" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K32" s="61">
+        <v>120</v>
       </c>
       <c r="L32" s="61">
         <v>120</v>
       </c>
       <c r="M32" s="61">
+        <v>100</v>
+      </c>
+      <c r="N32" s="61">
+        <v>100</v>
+      </c>
+      <c r="O32" s="61">
         <v>120</v>
       </c>
-      <c r="N32" s="61">
-        <v>100</v>
-      </c>
-      <c r="O32" s="61">
-        <v>100</v>
-      </c>
       <c r="P32" s="61">
+        <v>150</v>
+      </c>
+      <c r="Q32" s="61">
+        <v>170</v>
+      </c>
+      <c r="R32" s="61">
+        <v>200</v>
+      </c>
+      <c r="S32" s="61">
+        <v>170</v>
+      </c>
+      <c r="T32" s="61">
+        <v>200</v>
+      </c>
+      <c r="U32" s="61">
+        <v>150</v>
+      </c>
+      <c r="V32" s="61">
+        <v>200</v>
+      </c>
+      <c r="W32" s="61">
         <v>120</v>
       </c>
-      <c r="Q32" s="61">
-        <v>150</v>
-      </c>
-      <c r="R32" s="61">
-        <v>170</v>
-      </c>
-      <c r="S32" s="61">
-        <v>200</v>
-      </c>
-      <c r="T32" s="61">
-        <v>170</v>
-      </c>
-      <c r="U32" s="61">
-        <v>200</v>
-      </c>
-      <c r="V32" s="61">
-        <v>150</v>
-      </c>
-      <c r="W32" s="61">
-        <v>200</v>
-      </c>
       <c r="X32" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y32" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z32" s="61">
         <v>220</v>
       </c>
       <c r="AA32" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB32" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC32" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="57" t="s">
+      <c r="B33" s="57" t="s">
         <v>37</v>
       </c>
+      <c r="C33" s="58">
+        <v>51</v>
+      </c>
       <c r="D33" s="58">
-        <v>51</v>
+        <v>29.5</v>
       </c>
       <c r="E33" s="58">
-        <v>29.5</v>
-      </c>
-      <c r="F33" s="58">
         <v>33.299999999999997</v>
+      </c>
+      <c r="F33" s="62" t="s">
+        <v>50</v>
       </c>
       <c r="G33" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="62">
-        <v>250</v>
+      <c r="H33" s="62">
+        <v>250</v>
+      </c>
+      <c r="I33" s="56">
+        <v>100</v>
       </c>
       <c r="J33" s="56">
-        <v>100</v>
-      </c>
-      <c r="K33" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K33" s="62">
+        <v>120</v>
       </c>
       <c r="L33" s="62">
+        <v>150</v>
+      </c>
+      <c r="M33" s="61">
+        <v>100</v>
+      </c>
+      <c r="N33" s="61">
+        <v>100</v>
+      </c>
+      <c r="O33" s="62">
         <v>120</v>
       </c>
-      <c r="M33" s="62">
-        <v>150</v>
-      </c>
-      <c r="N33" s="61">
-        <v>100</v>
-      </c>
-      <c r="O33" s="61">
-        <v>100</v>
-      </c>
       <c r="P33" s="62">
+        <v>150</v>
+      </c>
+      <c r="Q33" s="61">
+        <v>170</v>
+      </c>
+      <c r="R33" s="61">
+        <v>200</v>
+      </c>
+      <c r="S33" s="61">
+        <v>170</v>
+      </c>
+      <c r="T33" s="61">
+        <v>200</v>
+      </c>
+      <c r="U33" s="61">
+        <v>150</v>
+      </c>
+      <c r="V33" s="61">
+        <v>200</v>
+      </c>
+      <c r="W33" s="61">
         <v>120</v>
       </c>
-      <c r="Q33" s="62">
-        <v>150</v>
-      </c>
-      <c r="R33" s="61">
-        <v>170</v>
-      </c>
-      <c r="S33" s="61">
-        <v>200</v>
-      </c>
-      <c r="T33" s="61">
-        <v>170</v>
-      </c>
-      <c r="U33" s="61">
-        <v>200</v>
-      </c>
-      <c r="V33" s="61">
-        <v>150</v>
-      </c>
-      <c r="W33" s="61">
-        <v>200</v>
-      </c>
       <c r="X33" s="61">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y33" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z33" s="61">
         <v>220</v>
       </c>
       <c r="AA33" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB33" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC33" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="57" t="s">
+      <c r="B34" s="57" t="s">
         <v>35</v>
       </c>
+      <c r="C34" s="58">
+        <v>60</v>
+      </c>
       <c r="D34" s="58">
-        <v>60</v>
+        <v>34.1</v>
       </c>
       <c r="E34" s="58">
-        <v>34.1</v>
-      </c>
-      <c r="F34" s="58">
         <v>39.4</v>
       </c>
-      <c r="G34" s="59">
+      <c r="F34" s="59">
         <v>1.17E-2</v>
       </c>
-      <c r="H34" s="60">
+      <c r="G34" s="60">
         <v>3.14</v>
       </c>
-      <c r="I34" s="61">
+      <c r="H34" s="61">
         <v>350</v>
       </c>
+      <c r="I34" s="56">
+        <v>100</v>
+      </c>
       <c r="J34" s="56">
-        <v>100</v>
-      </c>
-      <c r="K34" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K34" s="61">
+        <v>200</v>
       </c>
       <c r="L34" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M34" s="61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N34" s="61">
         <v>100</v>
       </c>
       <c r="O34" s="61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P34" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q34" s="61">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="R34" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S34" s="61">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="T34" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="U34" s="61">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="V34" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W34" s="61">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="X34" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="Y34" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z34" s="61">
         <v>220</v>
       </c>
       <c r="AA34" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB34" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC34" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="57" t="s">
+      <c r="B35" s="57" t="s">
         <v>43</v>
       </c>
+      <c r="C35" s="58">
+        <v>40</v>
+      </c>
       <c r="D35" s="58">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E35" s="58">
-        <v>18</v>
-      </c>
-      <c r="F35" s="58">
         <v>10.6</v>
       </c>
-      <c r="G35" s="59">
+      <c r="F35" s="59">
         <v>1.9900000000000001E-2</v>
       </c>
-      <c r="H35" s="60">
+      <c r="G35" s="60">
         <v>3.1070000000000002</v>
       </c>
-      <c r="I35" s="61">
+      <c r="H35" s="61">
         <v>350</v>
       </c>
+      <c r="I35" s="56">
+        <v>100</v>
+      </c>
       <c r="J35" s="56">
-        <v>100</v>
-      </c>
-      <c r="K35" s="56">
+        <v>180</v>
+      </c>
+      <c r="K35" s="61">
         <v>180</v>
       </c>
       <c r="L35" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M35" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N35" s="61">
         <v>100</v>
       </c>
       <c r="O35" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P35" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q35" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R35" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S35" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T35" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U35" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V35" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W35" s="61">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="X35" s="61">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="Y35" s="61">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="Z35" s="61">
         <v>220</v>
       </c>
       <c r="AA35" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB35" s="61">
         <v>300</v>
       </c>
-      <c r="AC35" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="57" t="s">
+      <c r="B36" s="57" t="s">
         <v>43</v>
       </c>
+      <c r="C36" s="58">
+        <v>40</v>
+      </c>
       <c r="D36" s="58">
-        <v>40</v>
+        <v>23.8</v>
       </c>
       <c r="E36" s="58">
-        <v>23.8</v>
-      </c>
-      <c r="F36" s="58">
         <v>26</v>
       </c>
+      <c r="F36" s="62">
+        <v>4.41E-2</v>
+      </c>
       <c r="G36" s="62">
-        <v>4.41E-2</v>
+        <v>2.597</v>
       </c>
       <c r="H36" s="62">
-        <v>2.597</v>
-      </c>
-      <c r="I36" s="62">
         <v>350</v>
       </c>
+      <c r="I36" s="56">
+        <v>100</v>
+      </c>
       <c r="J36" s="56">
-        <v>100</v>
-      </c>
-      <c r="K36" s="56">
+        <v>180</v>
+      </c>
+      <c r="K36" s="62">
         <v>180</v>
       </c>
       <c r="L36" s="62">
-        <v>180</v>
-      </c>
-      <c r="M36" s="62">
-        <v>200</v>
+        <v>200</v>
+      </c>
+      <c r="M36" s="61">
+        <v>100</v>
       </c>
       <c r="N36" s="61">
         <v>100</v>
       </c>
-      <c r="O36" s="61">
-        <v>100</v>
+      <c r="O36" s="62">
+        <v>230</v>
       </c>
       <c r="P36" s="62">
-        <v>230</v>
-      </c>
-      <c r="Q36" s="62">
         <v>270</v>
       </c>
+      <c r="Q36" s="61">
+        <v>170</v>
+      </c>
       <c r="R36" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S36" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T36" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U36" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V36" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W36" s="61">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="X36" s="61">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="Y36" s="61">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="Z36" s="61">
         <v>220</v>
       </c>
       <c r="AA36" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB36" s="61">
         <v>300</v>
       </c>
-      <c r="AC36" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="57" t="s">
+      <c r="B37" s="57" t="s">
         <v>43</v>
       </c>
+      <c r="C37" s="58">
+        <v>45</v>
+      </c>
       <c r="D37" s="58">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E37" s="58">
-        <v>26</v>
-      </c>
-      <c r="F37" s="58">
         <v>29.1</v>
       </c>
-      <c r="G37" s="59">
+      <c r="F37" s="59">
         <v>3.2800000000000003E-2</v>
       </c>
-      <c r="H37" s="60">
+      <c r="G37" s="60">
         <v>2.7160000000000002</v>
       </c>
-      <c r="I37" s="61">
+      <c r="H37" s="61">
         <v>350</v>
       </c>
+      <c r="I37" s="56">
+        <v>100</v>
+      </c>
       <c r="J37" s="56">
-        <v>100</v>
-      </c>
-      <c r="K37" s="56">
+        <v>180</v>
+      </c>
+      <c r="K37" s="61">
         <v>180</v>
       </c>
       <c r="L37" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="M37" s="61">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N37" s="61">
         <v>100</v>
       </c>
       <c r="O37" s="61">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="P37" s="61">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="Q37" s="61">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="R37" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S37" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="T37" s="61">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U37" s="61">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="V37" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W37" s="61">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="X37" s="61">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="Y37" s="61">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="Z37" s="61">
         <v>220</v>
       </c>
       <c r="AA37" s="61">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="AB37" s="61">
         <v>300</v>
       </c>
-      <c r="AC37" s="61">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="57" t="s">
+      <c r="B38" s="57" t="s">
         <v>44</v>
       </c>
+      <c r="C38" s="58">
+        <v>234</v>
+      </c>
       <c r="D38" s="58">
-        <v>234</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="E38" s="58">
-        <v>75.599999999999994</v>
-      </c>
-      <c r="F38" s="58">
         <v>108.9</v>
       </c>
-      <c r="G38" s="59">
+      <c r="F38" s="59">
         <v>1.4800000000000001E-2</v>
       </c>
-      <c r="H38" s="60">
+      <c r="G38" s="60">
         <v>2.97</v>
       </c>
-      <c r="I38" s="61">
-        <v>250</v>
+      <c r="H38" s="61">
+        <v>250</v>
+      </c>
+      <c r="I38" s="56">
+        <v>100</v>
       </c>
       <c r="J38" s="56">
-        <v>100</v>
-      </c>
-      <c r="K38" s="56">
-        <v>180</v>
+        <v>180</v>
+      </c>
+      <c r="K38" s="61">
+        <v>150</v>
       </c>
       <c r="L38" s="61">
         <v>150</v>
       </c>
       <c r="M38" s="61">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N38" s="61">
         <v>100</v>
       </c>
       <c r="O38" s="61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P38" s="61">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q38" s="61">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="R38" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="S38" s="61">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="T38" s="61">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="U38" s="61">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="V38" s="61">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="W38" s="61">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="X38" s="61">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="Y38" s="61">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="Z38" s="61">
         <v>220</v>
       </c>
       <c r="AA38" s="61">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="AB38" s="61">
-        <v>150</v>
-      </c>
-      <c r="AC38" s="61">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="42" spans="1:29" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+      <c r="K42" s="63"/>
       <c r="L42" s="63"/>
       <c r="M42" s="63"/>
       <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
+      <c r="O42" s="72"/>
       <c r="P42" s="72"/>
-      <c r="Q42" s="72"/>
+      <c r="Q42" s="64"/>
       <c r="R42" s="64"/>
-      <c r="S42" s="64"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L43" s="65"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L44" s="65"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L45" s="65"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L46" s="65"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L47" s="65"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K43" s="65"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K44" s="65"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K45" s="65"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K46" s="65"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K47" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6066,7 +5954,7 @@
   <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A40"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9313,7 +9201,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fishlandings output figures and expanding fishbase information
</commit_message>
<xml_diff>
--- a/FishLandings/output/statistics_v2.xlsx
+++ b/FishLandings/output/statistics_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4F4CF0-0FD4-EA42-BB1A-5A08E3810B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F07D0D-2EFE-5646-A62F-E3C58A4DED14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="460" windowWidth="27380" windowHeight="18580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="3720" windowWidth="27380" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Per Trap Stats" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
   <si>
     <t xml:space="preserve">t </t>
   </si>
@@ -335,32 +335,6 @@
   </si>
   <si>
     <r>
-      <t>Protein (g trap</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>VitaminA (ug trap</t>
     </r>
     <r>
@@ -438,30 +412,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Yield (kg trap</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Species Richness </t>
   </si>
   <si>
@@ -494,8 +444,83 @@
     <t>Yield (kg) Taken Home</t>
   </si>
   <si>
+    <t>Price (KES/kg)</t>
+  </si>
+  <si>
+    <r>
+      <t>CPUE (n trap</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Protein (g trap</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Bycatch (kg trap</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Yield (kg trap</t>
     </r>
     <r>
       <rPr>
@@ -518,9 +543,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Price (KES/kg)</t>
   </si>
 </sst>
 </file>
@@ -776,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -790,9 +812,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -836,9 +855,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -909,14 +925,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1232,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P25"/>
+  <dimension ref="B2:P28"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,227 +1278,159 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="2:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="46"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="44"/>
     </row>
     <row r="4" spans="2:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12">
-        <v>-0.89383000000000001</v>
-      </c>
-      <c r="G5" s="12">
-        <v>2651.7</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.3715</v>
-      </c>
+      <c r="B5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="52"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11">
-        <v>0.82654000000000005</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E6" s="14">
-        <v>2219</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="5"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="49"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="11">
-        <v>0.84311550000000002</v>
-      </c>
-      <c r="D7" s="11">
-        <v>1.407051E-2</v>
-      </c>
-      <c r="E7" s="14">
-        <v>1122</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="5"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="30">
-        <v>-5.9923000000000002</v>
-      </c>
-      <c r="G8" s="12">
-        <v>2066.1</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+    </row>
+    <row r="8" spans="2:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="B8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="11">
-        <v>27.190999999999999</v>
-      </c>
-      <c r="D9" s="11">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E9" s="14">
-        <v>2929</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="5"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="46"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="47"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10">
-        <v>28.018999999999998</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.115</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1089</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="5"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="46"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12">
-        <v>-5.2089999999999996</v>
-      </c>
-      <c r="G11" s="12">
-        <v>2084.9</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>59</v>
-      </c>
+      <c r="B11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="41"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="11">
-        <v>4.5556669999999997</v>
-      </c>
-      <c r="D12" s="11">
-        <v>3.4746480000000003E-2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2982</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="5"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1482,302 +1440,277 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="11">
-        <v>4.8883850000000004</v>
-      </c>
-      <c r="D13" s="11">
-        <v>5.359618E-2</v>
-      </c>
-      <c r="E13" s="14">
-        <v>1102</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="5"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="46"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12">
-        <v>-2.7246000000000001</v>
-      </c>
-      <c r="G14" s="12">
-        <v>2464.9</v>
-      </c>
-      <c r="H14" s="25">
-        <v>6.4840000000000002E-3</v>
-      </c>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B14" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="41"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="46"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="44"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="11">
-        <v>159.14179999999999</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2.2397659999999999</v>
-      </c>
-      <c r="E15" s="14">
-        <v>2181</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="5"/>
-      <c r="J15" s="47"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="49"/>
+      <c r="P15" s="3"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="11">
-        <v>168.982</v>
-      </c>
-      <c r="D16" s="11">
-        <v>2.8332709999999999</v>
-      </c>
-      <c r="E16" s="14">
-        <v>1122</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="5"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="46"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="44"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12">
-        <v>-7.0563000000000002</v>
-      </c>
-      <c r="G17" s="12">
-        <v>987.66</v>
-      </c>
-      <c r="H17" s="43" t="s">
-        <v>59</v>
-      </c>
+    <row r="17" spans="2:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="53"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="46"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="44"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="11">
-        <v>3.9888460000000001</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0.16762589999999999</v>
-      </c>
-      <c r="E18" s="14">
-        <v>1638</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="5"/>
-      <c r="J18" s="47"/>
+      <c r="J18" s="45"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="50"/>
+      <c r="P18" s="47"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="11">
-        <v>6.749555</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0.35351110000000002</v>
-      </c>
-      <c r="E19" s="14">
-        <v>673</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="5"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="46"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
-        <v>-22.966999999999999</v>
-      </c>
-      <c r="G20" s="44">
-        <v>1446.8</v>
-      </c>
-      <c r="H20" s="43" t="s">
-        <v>59</v>
-      </c>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="41"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="46"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="26">
-        <v>134.4675</v>
-      </c>
-      <c r="D21" s="27">
-        <v>2.077728</v>
-      </c>
-      <c r="E21" s="14">
-        <v>2152</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="5"/>
-      <c r="J21" s="47"/>
+      <c r="J21" s="45"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="49"/>
+      <c r="P21" s="48"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="32">
-        <v>262.32749999999999</v>
-      </c>
-      <c r="D22" s="32">
-        <v>5.164847</v>
-      </c>
-      <c r="E22" s="18">
-        <v>1087</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="8"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="5"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="46"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
-        <v>-5.5231000000000003</v>
-      </c>
-      <c r="G23" s="44">
-        <v>504.67</v>
-      </c>
-      <c r="H23" s="43" t="s">
-        <v>59</v>
-      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="41"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="44"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="54">
-        <v>6.9290000000000004E-2</v>
-      </c>
-      <c r="D24" s="11">
-        <v>2.933607E-3</v>
-      </c>
-      <c r="E24" s="14">
-        <v>336</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="5"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="47"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="13">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="D25" s="13">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="E25" s="18">
-        <v>328</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="8"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="2:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="B26" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="41"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1791,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37B7C5C-CFF2-2B46-947D-C21CFEAA6F44}">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -1815,1297 +1748,1297 @@
       <c r="C2"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="33" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <v>23.2</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="36">
         <v>120</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="37">
         <v>45.309964273364997</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="37">
         <v>0.74512301712761897</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="37">
         <v>0.103115029053002</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="37">
         <v>18.6290434054402</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="37">
         <v>21.0123170004094</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="37">
         <v>21.764275640550899</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="37">
         <v>2.17017657826612</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="36">
         <v>7.8</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="36">
         <v>120</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="37">
         <v>90.128694221655394</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="37">
         <v>1.00928197980354</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="37">
         <v>0.119621467402985</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="37">
         <v>18.531417643400999</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="37">
         <v>27.514568928978399</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="37">
         <v>17.8830681418228</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="37">
         <v>2.8078100553300902</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="36">
         <v>12.3</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="36">
         <v>120</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="37">
         <v>93.289489805937805</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="37">
         <v>0.97781435977640296</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="37">
         <v>0.130899381344249</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="37">
         <v>19.022885281025602</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="37">
         <v>26.523050241289901</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="37">
         <v>20.328516486673202</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="37">
         <v>2.3490973494470602</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="36">
         <v>35.5</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="36">
         <v>120</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="37">
         <v>45.125820261321003</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="37">
         <v>0.69898280060935603</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="37">
         <v>0.12700550002998701</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="37">
         <v>19.381643352550299</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="37">
         <v>31.301348720118501</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="37">
         <v>26.6350714357188</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="37">
         <v>1.98681582925077</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="36">
         <v>39.299999999999997</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="36">
         <v>120</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="37">
         <v>23.3123895982893</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="37">
         <v>0.54038604106955501</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="37">
         <v>0.105656587310822</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="37">
         <v>19.092631766129301</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="37">
         <v>20.0205058754383</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="37">
         <v>47.578684283890901</v>
       </c>
-      <c r="L9" s="39">
+      <c r="L9" s="37">
         <v>1.12204275865179</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="36">
         <v>48.8</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="36">
         <v>120</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="37">
         <v>20.999077617428402</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="37">
         <v>0.41680868190592602</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="37">
         <v>0.11697684191959901</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="37">
         <v>19.093792050938699</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="37">
         <v>49.0886119267034</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="37">
         <v>40.005955975971801</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="37">
         <v>1.05469287708994</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="36">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="36">
         <v>80</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="39">
         <v>95.730234800000005</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="39">
         <v>0.82108724</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="39">
         <v>0.14622162</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="39">
         <v>19.450248800000001</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="39">
         <v>33.402357899999998</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="39">
         <v>33.804601699999999</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="39">
         <v>1.1832891400000001</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="36">
         <v>10.6</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="36">
         <v>80</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="37">
         <v>95.457044899125705</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="37">
         <v>0.89565850232670297</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="37">
         <v>0.132454026468284</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="37">
         <v>18.853117450835999</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="37">
         <v>35.074455849112802</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="37">
         <v>29.439336126348302</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="37">
         <v>1.4962083389363501</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="36">
         <v>13.5</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="36">
         <v>200</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="40">
         <v>252</v>
       </c>
-      <c r="G13" s="42">
+      <c r="G13" s="40">
         <v>1.82</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="40">
         <v>0.29299999999999998</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="40">
         <v>20.5</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="40">
         <v>32</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="40">
         <v>85.8</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="40">
         <v>1.17</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="36">
         <v>18.5</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="36">
         <v>260</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="37">
         <v>92.748303409605199</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="37">
         <v>1.1869638599052501</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="37">
         <v>0.27412707095546301</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="37">
         <v>18.204891738191201</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="37">
         <v>30.9153974387932</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="37">
         <v>40.083377478182101</v>
       </c>
-      <c r="L14" s="39">
+      <c r="L14" s="37">
         <v>1.8703748202989701</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="36">
         <v>34.1</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="36">
         <v>160</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="37">
         <v>36.227347737587998</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="37">
         <v>0.482351467787486</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="37">
         <v>0.139900155559221</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="37">
         <v>19.708254195587202</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="37">
         <v>79.073076056484297</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="37">
         <v>40.565107867856902</v>
       </c>
-      <c r="L15" s="39">
+      <c r="L15" s="37">
         <v>0.95214251803889705</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="36">
         <v>29</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="36">
         <v>160</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="37">
         <v>42.232819657671499</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="37">
         <v>0.51832918371075598</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="37">
         <v>0.144220565509624</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="37">
         <v>19.698163484733499</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="37">
         <v>81.613061199635695</v>
       </c>
-      <c r="K16" s="39">
+      <c r="K16" s="37">
         <v>39.407901685833401</v>
       </c>
-      <c r="L16" s="39">
+      <c r="L16" s="37">
         <v>1.0017128891579099</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="36">
         <v>34.1</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="36">
         <v>160</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="37">
         <v>42.419641871367702</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="37">
         <v>0.55182248079029095</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="37">
         <v>0.14074104787398201</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="37">
         <v>19.8594314751344</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="37">
         <v>55.668096521456</v>
       </c>
-      <c r="K17" s="39">
+      <c r="K17" s="37">
         <v>44.293083956652097</v>
       </c>
-      <c r="L17" s="39">
+      <c r="L17" s="37">
         <v>0.95504939507097497</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="36">
         <v>40</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="36">
         <v>160</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="40">
         <v>26.6</v>
       </c>
-      <c r="G18" s="42">
+      <c r="G18" s="40">
         <v>0.47299999999999998</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="40">
         <v>0.111</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="40">
         <v>19.399999999999999</v>
       </c>
-      <c r="J18" s="42">
+      <c r="J18" s="40">
         <v>70.3</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="40">
         <v>31.9</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="40">
         <v>1.05</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="36">
         <v>42</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="36">
         <v>200</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="37">
         <v>49.046885128427498</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="37">
         <v>0.96115139477101097</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="37">
         <v>0.17202208983980699</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="37">
         <v>20.039407235669302</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="37">
         <v>21.557417850572001</v>
       </c>
-      <c r="K19" s="39">
+      <c r="K19" s="37">
         <v>50.329098233314198</v>
       </c>
-      <c r="L19" s="39">
+      <c r="L19" s="37">
         <v>2.2525138073183699</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="36">
         <v>23.6</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="36">
         <v>200</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="37">
         <v>62.104418334950701</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="37">
         <v>1.2512488713901899</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="37">
         <v>0.26399375925047402</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="37">
         <v>19.2106591947854</v>
       </c>
-      <c r="J20" s="39">
+      <c r="J20" s="37">
         <v>19.069057383991101</v>
       </c>
-      <c r="K20" s="39">
+      <c r="K20" s="37">
         <v>49.912352254307997</v>
       </c>
-      <c r="L20" s="39">
+      <c r="L20" s="37">
         <v>2.8354304445087601</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="36">
         <v>35.200000000000003</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="36">
         <v>200</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="37">
         <v>27.363725833553001</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="37">
         <v>0.66036717822868196</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="37">
         <v>0.120917095529385</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="37">
         <v>20.0642902760117</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="37">
         <v>28.293897139240201</v>
       </c>
-      <c r="K21" s="39">
+      <c r="K21" s="37">
         <v>46.285646564663097</v>
       </c>
-      <c r="L21" s="39">
+      <c r="L21" s="37">
         <v>2.0495681063004199</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="36">
         <v>37.4</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="36">
         <v>200</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="37">
         <v>38.016971002099503</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="37">
         <v>0.94532777745911201</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="37">
         <v>0.24694503319132199</v>
       </c>
-      <c r="I22" s="39">
+      <c r="I22" s="37">
         <v>19.267311246505798</v>
       </c>
-      <c r="J22" s="39">
+      <c r="J22" s="37">
         <v>21.2333912872821</v>
       </c>
-      <c r="K22" s="39">
+      <c r="K22" s="37">
         <v>53.478930246079599</v>
       </c>
-      <c r="L22" s="39">
+      <c r="L22" s="37">
         <v>2.3619518228279701</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="36">
         <v>34.1</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="36">
         <v>200</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="37">
         <v>14.8169028341455</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="37">
         <v>0.13482519745185201</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="37">
         <v>6.6892835287656202E-2</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="37">
         <v>19.812103002273901</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="37">
         <v>49.421730526725298</v>
       </c>
-      <c r="K23" s="39">
+      <c r="K23" s="37">
         <v>75.489675290439905</v>
       </c>
-      <c r="L23" s="39">
+      <c r="L23" s="37">
         <v>0.44841391270958297</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="36">
         <v>13.6</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="36">
         <v>200</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="37">
         <v>59.780760398709099</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="37">
         <v>0.54553773932259098</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="37">
         <v>0.30404417564292602</v>
       </c>
-      <c r="I24" s="39">
+      <c r="I24" s="37">
         <v>17.6267018771244</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="37">
         <v>134.55494646341199</v>
       </c>
-      <c r="K24" s="39">
+      <c r="K24" s="37">
         <v>71.026789131378905</v>
       </c>
-      <c r="L24" s="39">
+      <c r="L24" s="37">
         <v>0.75281587176924802</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="36">
         <v>12.5</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="36">
         <v>80</v>
       </c>
-      <c r="F25" s="39">
+      <c r="F25" s="37">
         <v>37.348952068405701</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="37">
         <v>1.08801456057672</v>
       </c>
-      <c r="H25" s="39">
+      <c r="H25" s="37">
         <v>8.1695664055271594E-2</v>
       </c>
-      <c r="I25" s="39">
+      <c r="I25" s="37">
         <v>18.335216998795499</v>
       </c>
-      <c r="J25" s="39">
+      <c r="J25" s="37">
         <v>49.683832871336797</v>
       </c>
-      <c r="K25" s="39">
+      <c r="K25" s="37">
         <v>36.442683403827203</v>
       </c>
-      <c r="L25" s="39">
+      <c r="L25" s="37">
         <v>1.91540635428554</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="36">
         <v>19.899999999999999</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="36">
         <v>160</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="37">
         <v>44.393490804576899</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="37">
         <v>0.49121594589897899</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="37">
         <v>0.158969400413628</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="37">
         <v>19.037684683597099</v>
       </c>
-      <c r="J26" s="39">
+      <c r="J26" s="37">
         <v>86.8299758561065</v>
       </c>
-      <c r="K26" s="39">
+      <c r="K26" s="37">
         <v>38.954418773752998</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="37">
         <v>1.0287260765670201</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="36">
         <v>17.5</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E27" s="36">
         <v>160</v>
       </c>
-      <c r="F27" s="39">
+      <c r="F27" s="37">
         <v>40.792371675731601</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="37">
         <v>0.36458854597025098</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="37">
         <v>0.24347963650617099</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="37">
         <v>16.895399498660201</v>
       </c>
-      <c r="J27" s="39">
+      <c r="J27" s="37">
         <v>408.27656824723601</v>
       </c>
-      <c r="K27" s="39">
+      <c r="K27" s="37">
         <v>53.654997396381802</v>
       </c>
-      <c r="L27" s="39">
+      <c r="L27" s="37">
         <v>0.748832320762016</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="36">
         <v>26.5</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="36">
         <v>160</v>
       </c>
-      <c r="F28" s="39">
+      <c r="F28" s="37">
         <v>40.068046781272102</v>
       </c>
-      <c r="G28" s="39">
+      <c r="G28" s="37">
         <v>0.38255663328151901</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="37">
         <v>0.23922663189688201</v>
       </c>
-      <c r="I28" s="39">
+      <c r="I28" s="37">
         <v>17.107481328637601</v>
       </c>
-      <c r="J28" s="39">
+      <c r="J28" s="37">
         <v>294.042880323269</v>
       </c>
-      <c r="K28" s="39">
+      <c r="K28" s="37">
         <v>60.589776427807699</v>
       </c>
-      <c r="L28" s="39">
+      <c r="L28" s="37">
         <v>0.69595004469550104</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="36">
         <v>23.8</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="36">
         <v>160</v>
       </c>
-      <c r="F29" s="39">
+      <c r="F29" s="37">
         <v>34.6150610404069</v>
       </c>
-      <c r="G29" s="39">
+      <c r="G29" s="37">
         <v>0.31053499468671503</v>
       </c>
-      <c r="H29" s="39">
+      <c r="H29" s="37">
         <v>0.122357198639165</v>
       </c>
-      <c r="I29" s="39">
+      <c r="I29" s="37">
         <v>18.301797676740701</v>
       </c>
-      <c r="J29" s="39">
+      <c r="J29" s="37">
         <v>233.59456281711999</v>
       </c>
-      <c r="K29" s="39">
+      <c r="K29" s="37">
         <v>63.086143118770302</v>
       </c>
-      <c r="L29" s="39">
+      <c r="L29" s="37">
         <v>0.545369799017695</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="36">
         <v>30</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="36">
         <v>120</v>
       </c>
-      <c r="F30" s="39">
+      <c r="F30" s="37">
         <v>24.961328724718399</v>
       </c>
-      <c r="G30" s="39">
+      <c r="G30" s="37">
         <v>0.54765114878300802</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="37">
         <v>9.4229096274829199E-2</v>
       </c>
-      <c r="I30" s="39">
+      <c r="I30" s="37">
         <v>18.694330972080401</v>
       </c>
-      <c r="J30" s="39">
+      <c r="J30" s="37">
         <v>28.006734632678299</v>
       </c>
-      <c r="K30" s="39">
+      <c r="K30" s="37">
         <v>42.315135337144497</v>
       </c>
-      <c r="L30" s="39">
+      <c r="L30" s="37">
         <v>1.3279146263746</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D31" s="36">
         <v>21.3</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E31" s="36">
         <v>120</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="37">
         <v>51.183992609767998</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="37">
         <v>0.80292356446763502</v>
       </c>
-      <c r="H31" s="39">
+      <c r="H31" s="37">
         <v>0.107325650406506</v>
       </c>
-      <c r="I31" s="39">
+      <c r="I31" s="37">
         <v>18.735993165809202</v>
       </c>
-      <c r="J31" s="39">
+      <c r="J31" s="37">
         <v>25.349877493143399</v>
       </c>
-      <c r="K31" s="39">
+      <c r="K31" s="37">
         <v>38.645300073183897</v>
       </c>
-      <c r="L31" s="39">
+      <c r="L31" s="37">
         <v>1.63748685817832</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D32" s="36">
         <v>41.5</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="36">
         <v>120</v>
       </c>
-      <c r="F32" s="39">
+      <c r="F32" s="37">
         <v>32.352860890288802</v>
       </c>
-      <c r="G32" s="39">
+      <c r="G32" s="37">
         <v>0.91349242472560899</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="37">
         <v>0.166304769181086</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="37">
         <v>17.649409827034599</v>
       </c>
-      <c r="J32" s="39">
+      <c r="J32" s="37">
         <v>22.903536077872499</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32" s="37">
         <v>21.632748487537899</v>
       </c>
-      <c r="L32" s="39">
+      <c r="L32" s="37">
         <v>2.5772821702836701</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="36">
         <v>15.8</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="36">
         <v>120</v>
       </c>
-      <c r="F33" s="39">
+      <c r="F33" s="37">
         <v>58.8469132504774</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="37">
         <v>1.0819556724377</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="37">
         <v>9.5735866314246895E-2</v>
       </c>
-      <c r="I33" s="39">
+      <c r="I33" s="37">
         <v>18.977749682305799</v>
       </c>
-      <c r="J33" s="39">
+      <c r="J33" s="37">
         <v>13.7472945797532</v>
       </c>
-      <c r="K33" s="39">
+      <c r="K33" s="37">
         <v>21.6183163873269</v>
       </c>
-      <c r="L33" s="39">
+      <c r="L33" s="37">
         <v>2.44737616572933</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="36">
         <v>26.3</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="36">
         <v>120</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="37">
         <v>31.095357523903701</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="37">
         <v>0.79163962844298097</v>
       </c>
-      <c r="H34" s="39">
+      <c r="H34" s="37">
         <v>8.5113160472975902E-2</v>
       </c>
-      <c r="I34" s="39">
+      <c r="I34" s="37">
         <v>18.962856100310599</v>
       </c>
-      <c r="J34" s="39">
+      <c r="J34" s="37">
         <v>13.6450703244957</v>
       </c>
-      <c r="K34" s="39">
+      <c r="K34" s="37">
         <v>23.943160826380101</v>
       </c>
-      <c r="L34" s="39">
+      <c r="L34" s="37">
         <v>2.0036646307277599</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="36">
         <v>29.5</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="36">
         <v>120</v>
       </c>
-      <c r="F35" s="39">
+      <c r="F35" s="37">
         <v>33.210346908585997</v>
       </c>
-      <c r="G35" s="39">
+      <c r="G35" s="37">
         <v>0.76423279346481998</v>
       </c>
-      <c r="H35" s="39">
+      <c r="H35" s="37">
         <v>8.8909524098091205E-2</v>
       </c>
-      <c r="I35" s="39">
+      <c r="I35" s="37">
         <v>18.782030621089699</v>
       </c>
-      <c r="J35" s="39">
+      <c r="J35" s="37">
         <v>22.117286204210099</v>
       </c>
-      <c r="K35" s="39">
+      <c r="K35" s="37">
         <v>20.5665948582851</v>
       </c>
-      <c r="L35" s="39">
+      <c r="L35" s="37">
         <v>2.1754935639908801</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="36">
         <v>34.1</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="36">
         <v>200</v>
       </c>
-      <c r="F36" s="39">
+      <c r="F36" s="37">
         <v>35.918126538378203</v>
       </c>
-      <c r="G36" s="39">
+      <c r="G36" s="37">
         <v>0.52224557178557796</v>
       </c>
-      <c r="H36" s="39">
+      <c r="H36" s="37">
         <v>0.16657183543270501</v>
       </c>
-      <c r="I36" s="39">
+      <c r="I36" s="37">
         <v>18.650542506680399</v>
       </c>
-      <c r="J36" s="39">
+      <c r="J36" s="37">
         <v>167.921198602717</v>
       </c>
-      <c r="K36" s="39">
+      <c r="K36" s="37">
         <v>41.649657282384403</v>
       </c>
-      <c r="L36" s="39">
+      <c r="L36" s="37">
         <v>0.69011835922439702</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="36">
         <v>18</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="36">
         <v>200</v>
       </c>
-      <c r="F37" s="39">
+      <c r="F37" s="37">
         <v>82.284168226043406</v>
       </c>
-      <c r="G37" s="39">
+      <c r="G37" s="37">
         <v>1.3617634143717099</v>
       </c>
-      <c r="H37" s="39">
+      <c r="H37" s="37">
         <v>0.30869819444667101</v>
       </c>
-      <c r="I37" s="39">
+      <c r="I37" s="37">
         <v>18.7864510193135</v>
       </c>
-      <c r="J37" s="39">
+      <c r="J37" s="37">
         <v>12.5340073222137</v>
       </c>
-      <c r="K37" s="39">
+      <c r="K37" s="37">
         <v>26.5356572835164</v>
       </c>
-      <c r="L37" s="39">
+      <c r="L37" s="37">
         <v>1.6533738466419701</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D38" s="36">
         <v>23.8</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="36">
         <v>200</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="37">
         <v>35.722767695077899</v>
       </c>
-      <c r="G38" s="39">
+      <c r="G38" s="37">
         <v>0.63585327835814498</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="37">
         <v>0.13488215698967401</v>
       </c>
-      <c r="I38" s="39">
+      <c r="I38" s="37">
         <v>19.241489508897899</v>
       </c>
-      <c r="J38" s="39">
+      <c r="J38" s="37">
         <v>22.804239362941701</v>
       </c>
-      <c r="K38" s="39">
+      <c r="K38" s="37">
         <v>18.086912694931598</v>
       </c>
-      <c r="L38" s="39">
+      <c r="L38" s="37">
         <v>1.0995961849890099</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="36">
         <v>26</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="36">
         <v>200</v>
       </c>
-      <c r="F39" s="39">
+      <c r="F39" s="37">
         <v>43.740388503572603</v>
       </c>
-      <c r="G39" s="39">
+      <c r="G39" s="37">
         <v>0.93003884538987303</v>
       </c>
-      <c r="H39" s="39">
+      <c r="H39" s="37">
         <v>0.27535275590789798</v>
       </c>
-      <c r="I39" s="39">
+      <c r="I39" s="37">
         <v>18.198679865388801</v>
       </c>
-      <c r="J39" s="39">
+      <c r="J39" s="37">
         <v>26.982288317907699</v>
       </c>
-      <c r="K39" s="39">
+      <c r="K39" s="37">
         <v>21.138213788809601</v>
       </c>
-      <c r="L39" s="39">
+      <c r="L39" s="37">
         <v>1.70561291920585</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="38">
+      <c r="D40" s="36">
         <v>75.599999999999994</v>
       </c>
-      <c r="E40" s="38">
+      <c r="E40" s="36">
         <v>175</v>
       </c>
-      <c r="F40" s="39">
+      <c r="F40" s="37">
         <v>100</v>
       </c>
-      <c r="G40" s="39">
+      <c r="G40" s="37">
         <v>1.23</v>
       </c>
-      <c r="H40" s="39">
+      <c r="H40" s="37">
         <v>0.25600000000000001</v>
       </c>
-      <c r="I40" s="39">
+      <c r="I40" s="37">
         <v>19.399999999999999</v>
       </c>
-      <c r="J40" s="39">
+      <c r="J40" s="37">
         <v>3.29</v>
       </c>
-      <c r="K40" s="39">
+      <c r="K40" s="37">
         <v>173</v>
       </c>
-      <c r="L40" s="39">
+      <c r="L40" s="37">
         <v>0.85499999999999998</v>
       </c>
     </row>
@@ -3134,59 +3067,59 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
     </row>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
     </row>
     <row r="6" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="15">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="14">
         <v>-23.018999999999998</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="24">
         <v>1475.4</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -3194,293 +3127,293 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="24">
         <v>314.94619999999998</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <v>4.9803290000000002</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>2152</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>612.35900000000004</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <v>11.921783</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>1087</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="30">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="28">
         <v>-24.007999999999999</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="27">
         <v>1445.1</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <v>6.3630389999999997</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <v>9.7603750000000003E-2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>2152</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>12.654658</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <v>0.24320900000000001</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>1087</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="30">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="28">
         <v>-24.384</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="27">
         <v>1408.1</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="25">
         <v>1.631186</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="25">
         <v>2.550471E-2</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>2152</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="25">
         <v>3.380576</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="25">
         <v>6.7057199999999997E-2</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <v>1087</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11">
+        <v>-19.033000000000001</v>
+      </c>
+      <c r="G16" s="27">
+        <v>1437.9</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="24">
+        <v>215.12039999999999</v>
+      </c>
+      <c r="D17" s="25">
+        <v>3.4064019999999999</v>
+      </c>
+      <c r="E17" s="13">
+        <v>2152</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="25">
+        <v>390.6977</v>
+      </c>
+      <c r="D18" s="25">
+        <v>8.5730310000000003</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1087</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B19" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11">
+        <v>-16.675000000000001</v>
+      </c>
+      <c r="G19" s="27">
+        <v>1334.8</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="24">
+        <v>263.93729999999999</v>
+      </c>
+      <c r="D20" s="25">
+        <v>5.1196219999999997</v>
+      </c>
+      <c r="E20" s="13">
+        <v>2152</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="30">
+        <v>532.75130000000001</v>
+      </c>
+      <c r="D21" s="30">
+        <v>15.285924</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1087</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B22" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12">
-        <v>-19.033000000000001</v>
-      </c>
-      <c r="G16" s="29">
-        <v>1437.9</v>
-      </c>
-      <c r="H16" s="19" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11">
+        <v>-23.809000000000001</v>
+      </c>
+      <c r="G22" s="27">
+        <v>1450.5</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="51" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="26">
-        <v>215.12039999999999</v>
-      </c>
-      <c r="D17" s="27">
-        <v>3.4064019999999999</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="C23" s="10">
+        <v>12.990209999999999</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.19587199999999999</v>
+      </c>
+      <c r="E23" s="13">
         <v>2152</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="51" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="27">
-        <v>390.6977</v>
-      </c>
-      <c r="D18" s="27">
-        <v>8.5730310000000003</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="C24" s="12">
+        <v>25.431260000000002</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.48442819999999998</v>
+      </c>
+      <c r="E24" s="17">
         <v>1087</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12">
-        <v>-16.675000000000001</v>
-      </c>
-      <c r="G19" s="29">
-        <v>1334.8</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="26">
-        <v>263.93729999999999</v>
-      </c>
-      <c r="D20" s="27">
-        <v>5.1196219999999997</v>
-      </c>
-      <c r="E20" s="14">
-        <v>2152</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="32">
-        <v>532.75130000000001</v>
-      </c>
-      <c r="D21" s="32">
-        <v>15.285924</v>
-      </c>
-      <c r="E21" s="14">
-        <v>1087</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B22" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12">
-        <v>-23.809000000000001</v>
-      </c>
-      <c r="G22" s="29">
-        <v>1450.5</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="11">
-        <v>12.990209999999999</v>
-      </c>
-      <c r="D23" s="11">
-        <v>0.19587199999999999</v>
-      </c>
-      <c r="E23" s="14">
-        <v>2152</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="13">
-        <v>25.431260000000002</v>
-      </c>
-      <c r="D24" s="13">
-        <v>0.48442819999999998</v>
-      </c>
-      <c r="E24" s="18">
-        <v>1087</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="8"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed output from group by id and trap type
</commit_message>
<xml_diff>
--- a/FishLandings/output/statistics_v2.xlsx
+++ b/FishLandings/output/statistics_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D87864-3886-A041-89D2-6A66F29F4A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB79DA0D-1DDA-5147-8E01-2DEDFD6A8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="1060" windowWidth="24940" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6580" yWindow="11460" windowWidth="24940" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Per Trap Stats" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t xml:space="preserve">t </t>
   </si>
@@ -153,32 +153,6 @@
   <si>
     <r>
       <t>VitaminA (ug trap</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Selenium (ug trap</t>
     </r>
     <r>
       <rPr>
@@ -920,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -930,9 +904,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -962,9 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1050,6 +1018,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1058,9 +1029,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1072,6 +1040,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1390,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="116" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,207 +1391,207 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="2:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9">
+      <c r="B5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8">
         <v>0.60851</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="56">
         <v>262.79000000000002</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="38">
         <v>0.54339999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>3.30721</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.1011388</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>591</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="58"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>3.1861109999999999</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.17139289999999999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>150</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="58"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="41">
-        <v>-5.1447000000000003</v>
-      </c>
-      <c r="G8" s="59">
-        <v>159.97999999999999</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>42</v>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="39">
+        <v>-3.2639999999999998</v>
+      </c>
+      <c r="G8" s="57">
+        <v>200.96</v>
+      </c>
+      <c r="H8" s="29">
+        <v>1.291E-3</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
-        <v>1.0068969999999999</v>
-      </c>
-      <c r="D9" s="9">
-        <v>3.8089999999999999E-2</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="C9" s="8">
+        <v>0.95704199999999995</v>
+      </c>
+      <c r="D9" s="8">
+        <v>3.3550000000000003E-2</v>
+      </c>
+      <c r="E9" s="7">
         <v>591</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="58"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="4"/>
-      <c r="J9" s="34"/>
+      <c r="J9" s="32"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="35"/>
+      <c r="N9" s="33"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="36"/>
+      <c r="P9" s="34"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9">
-        <v>2.0530279999999999</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.19974</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="C10" s="8">
+        <v>1.24776</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8.2506999999999997E-2</v>
+      </c>
+      <c r="E10" s="7">
         <v>150</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="58"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="4"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="41">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="39">
         <v>-38.104999999999997</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="57">
         <v>3592</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>42</v>
+      <c r="H11" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="J11" s="3"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>25.288260000000001</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>4.8770000000000001E-2</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>15396</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="58"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="4"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1618,68 +1601,68 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>29.65465</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>0.10369</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>2428</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="58"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="4"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="33"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="41">
-        <v>7.6337999999999999</v>
-      </c>
-      <c r="G14" s="59">
-        <v>739</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>42</v>
+      <c r="B14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="39">
+        <v>18.172999999999998</v>
+      </c>
+      <c r="G14" s="57">
+        <v>436.22</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="33"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="9">
-        <v>4.4246999999999996</v>
-      </c>
-      <c r="D15" s="9">
-        <v>8.7639999999999996E-2</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="C15" s="8">
+        <v>4.3756349999999999</v>
+      </c>
+      <c r="D15" s="8">
+        <v>8.7054999999999993E-2</v>
+      </c>
+      <c r="E15" s="11">
         <v>591</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="58"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1689,353 +1672,353 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="9">
-        <v>2.9666000000000001</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.15640999999999999</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="C16" s="8">
+        <v>2.0533299999999999</v>
+      </c>
+      <c r="D16" s="8">
+        <v>9.354403E-2</v>
+      </c>
+      <c r="E16" s="11">
         <v>150</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="58"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="4"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="33"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="41">
-        <v>-5.8941999999999997</v>
-      </c>
-      <c r="G17" s="59">
-        <v>160.80000000000001</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>42</v>
+      <c r="B17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="39">
+        <v>-4.8760000000000003</v>
+      </c>
+      <c r="G17" s="57">
+        <v>202.64</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="33"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="9">
-        <v>162.52930000000001</v>
-      </c>
-      <c r="D18" s="9">
-        <v>6.352773</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="C18" s="8">
+        <v>153.4384</v>
+      </c>
+      <c r="D18" s="8">
+        <v>5.5807000000000002</v>
+      </c>
+      <c r="E18" s="11">
         <v>591</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="58"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="56"/>
       <c r="H18" s="4"/>
-      <c r="J18" s="34"/>
+      <c r="J18" s="32"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="36"/>
+      <c r="P18" s="34"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="9">
-        <v>355.67750000000001</v>
-      </c>
-      <c r="D19" s="9">
-        <v>32.147199999999998</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="C19" s="8">
+        <v>224.74340000000001</v>
+      </c>
+      <c r="D19" s="8">
+        <v>13.516920000000001</v>
+      </c>
+      <c r="E19" s="11">
         <v>150</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="58"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="4"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="33"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="41">
-        <v>-3.1585000000000001</v>
-      </c>
-      <c r="G20" s="59">
-        <v>41.655999999999999</v>
-      </c>
-      <c r="H20" s="31">
-        <v>2.9489999999999998E-3</v>
+      <c r="B20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="39">
+        <v>-3.0569000000000002</v>
+      </c>
+      <c r="G20" s="57">
+        <v>41.628999999999998</v>
+      </c>
+      <c r="H20" s="29">
+        <v>3.8969999999999999E-3</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="33"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="9">
-        <v>16.3644</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.61719999999999997</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="C21" s="8">
+        <v>16.340730000000001</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.61769070000000004</v>
+      </c>
+      <c r="E21" s="11">
         <v>352</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="58"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="4"/>
-      <c r="J21" s="34"/>
+      <c r="J21" s="32"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="37"/>
+      <c r="P21" s="35"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="9">
-        <v>27.1846</v>
-      </c>
-      <c r="D22" s="9">
-        <v>3.3696799999999998</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="C22" s="8">
+        <v>26.872109999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>3.3893116000000001</v>
+      </c>
+      <c r="E22" s="11">
         <v>40</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="58"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="56"/>
       <c r="H22" s="4"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="33"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B23" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="41">
-        <v>-6.1424000000000003</v>
-      </c>
-      <c r="G23" s="59">
-        <v>169.72</v>
-      </c>
-      <c r="H23" s="31" t="s">
-        <v>42</v>
+      <c r="B23" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="39">
+        <v>-2.9051</v>
+      </c>
+      <c r="G23" s="57">
+        <v>206.42</v>
+      </c>
+      <c r="H23" s="29">
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="33"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="9">
-        <v>178.58349999999999</v>
-      </c>
-      <c r="D24" s="9">
-        <v>6.3132999999999999</v>
-      </c>
-      <c r="E24" s="12">
-        <v>588</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="58"/>
+      <c r="C24" s="8">
+        <v>173.54679999999999</v>
+      </c>
+      <c r="D24" s="8">
+        <v>6.1083999999999996</v>
+      </c>
+      <c r="E24" s="11">
+        <v>590</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="56"/>
       <c r="H24" s="4"/>
-      <c r="J24" s="34"/>
+      <c r="J24" s="32"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="36"/>
+      <c r="P24" s="34"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="11">
-        <v>313.17809999999997</v>
-      </c>
-      <c r="D25" s="11">
-        <v>20.983000000000001</v>
-      </c>
-      <c r="E25" s="16">
-        <v>144</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="6"/>
+      <c r="C25" s="10">
+        <v>217.5128</v>
+      </c>
+      <c r="D25" s="10">
+        <v>13.846769999999999</v>
+      </c>
+      <c r="E25" s="15">
+        <v>147</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="5"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="33"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="31"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B26" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="41">
-        <v>-1.4977</v>
-      </c>
-      <c r="G26" s="59">
-        <v>20.603000000000002</v>
-      </c>
-      <c r="H26" s="55">
-        <v>0.14940000000000001</v>
+      <c r="B26" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="39">
+        <v>-1.7276</v>
+      </c>
+      <c r="G26" s="57">
+        <v>27.716999999999999</v>
+      </c>
+      <c r="H26" s="63">
+        <v>9.5189999999999997E-2</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="33"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="9">
-        <v>0.46489000000000003</v>
-      </c>
-      <c r="D27" s="9">
-        <v>8.2733000000000001E-2</v>
-      </c>
-      <c r="E27" s="12">
+      <c r="C27" s="8">
+        <v>0.44339460000000003</v>
+      </c>
+      <c r="D27" s="8">
+        <v>7.51E-2</v>
+      </c>
+      <c r="E27" s="11">
         <v>93</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="58"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="56"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="11">
-        <v>0.82230300000000001</v>
-      </c>
-      <c r="D28" s="11">
-        <v>0.22384000000000001</v>
-      </c>
-      <c r="E28" s="16">
+      <c r="C28" s="10">
+        <v>0.7046</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.13120599999999999</v>
+      </c>
+      <c r="E28" s="15">
         <v>17</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="6"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="41">
+      <c r="B29" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="39">
         <v>-20.591999999999999</v>
       </c>
-      <c r="G29" s="59">
+      <c r="G29" s="57">
         <v>3596.2</v>
       </c>
-      <c r="H29" s="31" t="s">
-        <v>42</v>
+      <c r="H29" s="29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>1.1839</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <v>6.447E-2</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="11">
         <v>15382</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="58"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="56"/>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>4.2981999999999996</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <v>0.1368</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="15">
         <v>2428</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="6"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2049,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE17491E-AE3E-0847-8740-D1EE4E6F1D7A}">
   <dimension ref="B4:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,353 +2045,353 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13">
-        <v>-6.0279999999999996</v>
-      </c>
-      <c r="G7" s="23">
-        <v>172.85</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>42</v>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="12">
+        <v>-2.8325999999999998</v>
+      </c>
+      <c r="G7" s="21">
+        <v>735</v>
+      </c>
+      <c r="H7" s="59">
+        <v>4.7739999999999996E-3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="23">
-        <v>410.42630000000003</v>
-      </c>
-      <c r="D8" s="24">
-        <v>14.70082</v>
-      </c>
-      <c r="E8" s="12">
-        <v>588</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="C8" s="21">
+        <v>397.45159999999998</v>
+      </c>
+      <c r="D8" s="22">
+        <v>13.936959999999999</v>
+      </c>
+      <c r="E8" s="11">
+        <v>590</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="60"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="23">
-        <v>703.29960000000005</v>
-      </c>
-      <c r="D9" s="24">
-        <v>46.308039999999998</v>
-      </c>
-      <c r="E9" s="12">
-        <v>144</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4"/>
+      <c r="C9" s="21">
+        <v>487.65859999999998</v>
+      </c>
+      <c r="D9" s="22">
+        <v>30.695540000000001</v>
+      </c>
+      <c r="E9" s="11">
+        <v>147</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="27">
-        <v>-6.3952999999999998</v>
-      </c>
-      <c r="G10" s="26">
-        <v>171.04</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>42</v>
+      <c r="C10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="25">
+        <v>-3.5209999999999999</v>
+      </c>
+      <c r="G10" s="24">
+        <v>204.14</v>
+      </c>
+      <c r="H10" s="61">
+        <v>5.3019999999999999E-4</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="23">
-        <v>8.2256619999999998</v>
-      </c>
-      <c r="D11" s="24">
-        <v>0.30567</v>
-      </c>
-      <c r="E11" s="12">
-        <v>588</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="4"/>
+      <c r="C11" s="21">
+        <v>7.9473599999999998</v>
+      </c>
+      <c r="D11" s="22">
+        <v>0.28932999999999998</v>
+      </c>
+      <c r="E11" s="11">
+        <v>590</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="60"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="23">
-        <v>14.8673</v>
-      </c>
-      <c r="D12" s="24">
-        <v>0.99250000000000005</v>
-      </c>
-      <c r="E12" s="12">
-        <v>144</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="4"/>
+      <c r="C12" s="21">
+        <v>10.510439999999999</v>
+      </c>
+      <c r="D12" s="22">
+        <v>0.66796999999999995</v>
+      </c>
+      <c r="E12" s="11">
+        <v>147</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="60"/>
     </row>
     <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="27">
-        <v>-7.7062999999999997</v>
-      </c>
-      <c r="G13" s="26">
-        <v>168.76</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>42</v>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="25">
+        <v>-5.6810999999999998</v>
+      </c>
+      <c r="G13" s="24">
+        <v>200.86</v>
+      </c>
+      <c r="H13" s="61" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="23">
-        <v>1.919384</v>
-      </c>
-      <c r="D14" s="24">
-        <v>7.2300000000000003E-2</v>
-      </c>
-      <c r="E14" s="12">
-        <v>588</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="21">
+        <v>1.8394710000000001</v>
+      </c>
+      <c r="D14" s="22">
+        <v>6.7979999999999999E-2</v>
+      </c>
+      <c r="E14" s="11">
+        <v>590</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="23">
-        <v>3.8879000000000001</v>
-      </c>
-      <c r="D15" s="24">
-        <v>0.24490000000000001</v>
-      </c>
-      <c r="E15" s="12">
-        <v>144</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="4"/>
+      <c r="C15" s="21">
+        <v>2.8342999999999998</v>
+      </c>
+      <c r="D15" s="22">
+        <v>0.16138</v>
+      </c>
+      <c r="E15" s="11">
+        <v>147</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9">
+        <v>-1.2131000000000001</v>
+      </c>
+      <c r="G16" s="24">
+        <v>735</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.22550000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="21">
+        <v>284.74930000000001</v>
+      </c>
+      <c r="D17" s="22">
+        <v>10.86938</v>
+      </c>
+      <c r="E17" s="11">
+        <v>590</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="60"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="21">
+        <v>314.82089999999999</v>
+      </c>
+      <c r="D18" s="22">
+        <v>23.736499999999999</v>
+      </c>
+      <c r="E18" s="11">
+        <v>147</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="60"/>
+    </row>
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9">
+        <v>-2.1774</v>
+      </c>
+      <c r="G19" s="24">
+        <v>735</v>
+      </c>
+      <c r="H19" s="61">
+        <v>2.9770000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="21">
+        <v>319.702</v>
+      </c>
+      <c r="D20" s="22">
+        <v>12.700011</v>
+      </c>
+      <c r="E20" s="11">
+        <v>590</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="60"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="55">
+        <v>381.39269999999999</v>
+      </c>
+      <c r="D21" s="27">
+        <v>24.96791</v>
+      </c>
+      <c r="E21" s="11">
+        <v>147</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="62"/>
+    </row>
+    <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B22" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10">
-        <v>-4.7667999999999999</v>
-      </c>
-      <c r="G16" s="26">
-        <v>171.04</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9">
+        <v>-2.4091999999999998</v>
+      </c>
+      <c r="G22" s="24">
+        <v>204.27</v>
+      </c>
+      <c r="H22" s="61">
+        <v>1.687E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="23">
-        <v>290.64210000000003</v>
-      </c>
-      <c r="D17" s="24">
-        <v>10.954890000000001</v>
-      </c>
-      <c r="E17" s="12">
-        <v>588</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="38" t="s">
+      <c r="C23" s="21">
+        <v>17.2135</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0.64012999999999998</v>
+      </c>
+      <c r="E23" s="11">
+        <v>590</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="60"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="23">
-        <v>426.82240000000002</v>
-      </c>
-      <c r="D18" s="24">
-        <v>35.568530000000003</v>
-      </c>
-      <c r="E18" s="12">
-        <v>144</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10">
-        <v>-5.5247999999999999</v>
-      </c>
-      <c r="G19" s="26">
-        <v>170.74</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="23">
-        <v>328.19349999999997</v>
-      </c>
-      <c r="D20" s="24">
-        <v>12.61805</v>
-      </c>
-      <c r="E20" s="12">
-        <v>588</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="57">
-        <v>566.15700000000004</v>
-      </c>
-      <c r="D21" s="29">
-        <v>41.182200000000002</v>
-      </c>
-      <c r="E21" s="12">
-        <v>144</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10">
-        <v>-5.5335999999999999</v>
-      </c>
-      <c r="G22" s="26">
-        <v>170.12</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="23">
-        <v>17.697399999999998</v>
-      </c>
-      <c r="D23" s="24">
-        <v>0.66559999999999997</v>
-      </c>
-      <c r="E23" s="12">
-        <v>588</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="57">
-        <v>30.398599999999998</v>
-      </c>
-      <c r="D24" s="29">
-        <v>2.19665</v>
-      </c>
-      <c r="E24" s="16">
-        <v>144</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="6"/>
+      <c r="C24" s="55">
+        <v>21.090299999999999</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1.4762999999999999</v>
+      </c>
+      <c r="E24" s="15">
+        <v>147</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2422,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9E1C08-A7E9-C84F-8ABE-E7EF96EBA4D4}">
   <dimension ref="B3:I21"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A11" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2433,7 +2416,7 @@
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="2" bestFit="1" customWidth="1"/>
@@ -2441,452 +2424,452 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" spans="2:9" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="52"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-    </row>
-    <row r="4" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-    </row>
-    <row r="5" spans="2:9" ht="19" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48" t="s">
+      <c r="D6" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="53"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="45" t="s">
+    </row>
+    <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="47">
+        <v>0.72887999999999997</v>
+      </c>
+      <c r="D7" s="48">
+        <v>149</v>
+      </c>
+      <c r="E7" s="48">
+        <v>590</v>
+      </c>
+      <c r="F7" s="50">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="G7" s="47">
+        <v>0.57044059999999996</v>
+      </c>
+      <c r="H7" s="47">
+        <v>0.94976649999999996</v>
+      </c>
+      <c r="I7" s="47">
+        <v>0.72887690000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="D8" s="48">
+        <v>149</v>
+      </c>
+      <c r="E8" s="48">
+        <v>590</v>
+      </c>
+      <c r="F8" s="50">
+        <v>5.2970000000000003E-4</v>
+      </c>
+      <c r="G8" s="47">
+        <v>1.201322</v>
+      </c>
+      <c r="H8" s="47">
+        <v>2.0001639999999998</v>
+      </c>
+      <c r="I8" s="47">
+        <v>1.5349809999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="54">
+        <v>0.71281000000000005</v>
+      </c>
+      <c r="D9" s="28">
+        <v>2427</v>
+      </c>
+      <c r="E9" s="28">
+        <v>15395</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="54">
+        <v>0.67137999999999998</v>
+      </c>
+      <c r="H9" s="54">
+        <v>0.7578146</v>
+      </c>
+      <c r="I9" s="54">
+        <v>0.7128101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="54">
+        <v>0.29304999999999998</v>
+      </c>
+      <c r="D10" s="28">
+        <v>149</v>
+      </c>
+      <c r="E10" s="28">
+        <v>590</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="54">
+        <v>0.22935</v>
+      </c>
+      <c r="H10" s="54">
+        <v>0.3818608</v>
+      </c>
+      <c r="I10" s="54">
+        <v>0.29305049999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B11" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="54">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="D11" s="28">
+        <v>149</v>
+      </c>
+      <c r="E11" s="28">
+        <v>590</v>
+      </c>
+      <c r="F11" s="53">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G11" s="54">
+        <v>1.1653009999999999</v>
+      </c>
+      <c r="H11" s="54">
+        <v>1.9401919999999999</v>
+      </c>
+      <c r="I11" s="54">
+        <v>1.4889570000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="54">
+        <v>3.4214000000000002</v>
+      </c>
+      <c r="D12" s="28">
+        <v>39</v>
+      </c>
+      <c r="E12" s="28">
+        <v>351</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="54">
+        <v>2.2290230000000002</v>
+      </c>
+      <c r="H12" s="54">
+        <v>5.7458809999999998</v>
+      </c>
+      <c r="I12" s="54">
+        <v>3.4213550000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="54">
+        <v>1.2803</v>
+      </c>
+      <c r="D13" s="28">
+        <v>146</v>
+      </c>
+      <c r="E13" s="28">
+        <v>589</v>
+      </c>
+      <c r="F13" s="50">
+        <v>4.9910000000000003E-2</v>
+      </c>
+      <c r="G13" s="54">
+        <v>1</v>
+      </c>
+      <c r="H13" s="54">
+        <v>1.6722729999999999</v>
+      </c>
+      <c r="I13" s="54">
+        <v>1.2802640000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B14" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="54">
+        <v>0.55650999999999995</v>
+      </c>
+      <c r="D14" s="28">
+        <v>16</v>
+      </c>
+      <c r="E14" s="28">
+        <v>92</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.1842</v>
+      </c>
+      <c r="G14" s="54">
+        <v>0.28520699999999999</v>
+      </c>
+      <c r="H14" s="54">
+        <v>1.3372200000000001</v>
+      </c>
+      <c r="I14" s="54">
+        <v>0.55651170000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="49">
-        <v>0.72887999999999997</v>
-      </c>
-      <c r="D7" s="50">
-        <v>149</v>
-      </c>
-      <c r="E7" s="50">
-        <v>590</v>
-      </c>
-      <c r="F7" s="51">
-        <v>1.9599999999999999E-2</v>
-      </c>
-      <c r="G7" s="49">
-        <v>0.57044059999999996</v>
-      </c>
-      <c r="H7" s="49">
-        <v>0.94976649999999996</v>
-      </c>
-      <c r="I7" s="49">
-        <v>0.72887690000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="49">
-        <v>6.9775999999999998</v>
-      </c>
-      <c r="D8" s="50">
-        <v>149</v>
-      </c>
-      <c r="E8" s="50">
-        <v>590</v>
-      </c>
-      <c r="F8" s="54" t="s">
+      <c r="C15" s="54">
+        <v>1.2085999999999999</v>
+      </c>
+      <c r="D15" s="28">
+        <v>146</v>
+      </c>
+      <c r="E15" s="28">
+        <v>589</v>
+      </c>
+      <c r="F15" s="49">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="G15" s="54">
+        <v>0.94410550000000004</v>
+      </c>
+      <c r="H15" s="54">
+        <v>1.5786553999999999</v>
+      </c>
+      <c r="I15" s="54">
+        <v>1.2085920000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B16" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="54">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="D16" s="28">
+        <v>146</v>
+      </c>
+      <c r="E16" s="28">
+        <v>589</v>
+      </c>
+      <c r="F16" s="50">
+        <v>2.4129999999999999E-2</v>
+      </c>
+      <c r="G16" s="54">
+        <v>1.0373000000000001</v>
+      </c>
+      <c r="H16" s="54">
+        <v>1.7345999999999999</v>
+      </c>
+      <c r="I16" s="54">
+        <v>1.3279810000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B17" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="54">
+        <v>1.4037999999999999</v>
+      </c>
+      <c r="D17" s="28">
+        <v>146</v>
+      </c>
+      <c r="E17" s="28">
+        <v>589</v>
+      </c>
+      <c r="F17" s="50">
+        <v>6.829E-3</v>
+      </c>
+      <c r="G17" s="54">
+        <v>1.0965800000000001</v>
+      </c>
+      <c r="H17" s="54">
+        <v>1.8335999999999999</v>
+      </c>
+      <c r="I17" s="54">
+        <v>1.40378</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="54">
+        <v>1.1881999999999999</v>
+      </c>
+      <c r="D18" s="28">
+        <v>146</v>
+      </c>
+      <c r="E18" s="28">
+        <v>589</v>
+      </c>
+      <c r="F18" s="48">
+        <v>0.17169999999999999</v>
+      </c>
+      <c r="G18" s="54">
+        <v>0.928176</v>
+      </c>
+      <c r="H18" s="54">
+        <v>1.552019</v>
+      </c>
+      <c r="I18" s="54">
+        <v>1.188199</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B19" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="54">
+        <v>0.96296999999999999</v>
+      </c>
+      <c r="D19" s="28">
+        <v>146</v>
+      </c>
+      <c r="E19" s="28">
+        <v>589</v>
+      </c>
+      <c r="F19" s="48">
+        <v>0.79410000000000003</v>
+      </c>
+      <c r="G19" s="54">
+        <v>0.75223839999999997</v>
+      </c>
+      <c r="H19" s="54">
+        <v>1.2578311</v>
+      </c>
+      <c r="I19" s="54">
+        <v>0.962974</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="54">
+        <v>1.3251999999999999</v>
+      </c>
+      <c r="D20" s="28">
+        <v>146</v>
+      </c>
+      <c r="E20" s="28">
+        <v>589</v>
+      </c>
+      <c r="F20" s="53">
+        <v>2.52E-2</v>
+      </c>
+      <c r="G20" s="54">
+        <v>1.035229</v>
+      </c>
+      <c r="H20" s="54">
+        <v>1.731025</v>
+      </c>
+      <c r="I20" s="54">
+        <v>1.3252429999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="49">
-        <v>5.4607999999999999</v>
-      </c>
-      <c r="H8" s="49">
-        <v>9.2219999999999996E-2</v>
-      </c>
-      <c r="I8" s="49">
-        <v>6.9776199999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="56">
-        <v>0.71281000000000005</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="C21" s="54">
+        <v>0.71106999999999998</v>
+      </c>
+      <c r="D21" s="28">
         <v>2427</v>
       </c>
-      <c r="E9" s="30">
-        <v>15395</v>
-      </c>
-      <c r="F9" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="56">
-        <v>0.67137999999999998</v>
-      </c>
-      <c r="H9" s="56">
-        <v>0.7578146</v>
-      </c>
-      <c r="I9" s="56">
-        <v>0.7128101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="56">
-        <v>0.80844000000000005</v>
-      </c>
-      <c r="D10" s="30">
-        <v>149</v>
-      </c>
-      <c r="E10" s="30">
-        <v>590</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0.11459999999999999</v>
-      </c>
-      <c r="G10" s="56">
-        <v>0.63270550000000003</v>
-      </c>
-      <c r="H10" s="56">
-        <v>1.0534357000000001</v>
-      </c>
-      <c r="I10" s="56">
-        <v>0.80843549999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="56">
-        <v>6.4992999999999999</v>
-      </c>
-      <c r="D11" s="30">
-        <v>149</v>
-      </c>
-      <c r="E11" s="30">
-        <v>590</v>
-      </c>
-      <c r="F11" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="56">
-        <v>5.0865200000000002</v>
-      </c>
-      <c r="H11" s="56">
-        <v>8.4689180000000004</v>
-      </c>
-      <c r="I11" s="56">
-        <v>6.4993809999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="56">
-        <v>3.3864999999999998</v>
-      </c>
-      <c r="D12" s="30">
-        <v>39</v>
-      </c>
-      <c r="E12" s="30">
-        <v>351</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="56">
-        <v>2.2062849999999998</v>
-      </c>
-      <c r="H12" s="56">
-        <v>5.6872689999999997</v>
-      </c>
-      <c r="I12" s="56">
-        <v>3.3864559999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="56">
-        <v>2.7052</v>
-      </c>
-      <c r="D13" s="30">
-        <v>143</v>
-      </c>
-      <c r="E13" s="30">
-        <v>587</v>
-      </c>
-      <c r="F13" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="56">
-        <v>2.1090469999999999</v>
-      </c>
-      <c r="H13" s="56">
-        <v>3.5425149999999999</v>
-      </c>
-      <c r="I13" s="56">
-        <v>2.7052489999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="56">
-        <v>1.3381000000000001</v>
-      </c>
-      <c r="D14" s="30">
-        <v>16</v>
-      </c>
-      <c r="E14" s="30">
-        <v>92</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0.38350000000000001</v>
-      </c>
-      <c r="G14" s="56">
-        <v>0.68569999999999998</v>
-      </c>
-      <c r="H14" s="56">
-        <v>3.2152599999999998</v>
-      </c>
-      <c r="I14" s="56">
-        <v>1.3380970000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="56">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="D15" s="30">
-        <v>143</v>
-      </c>
-      <c r="E15" s="30">
-        <v>587</v>
-      </c>
-      <c r="F15" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="56">
-        <v>1.894498</v>
-      </c>
-      <c r="H15" s="56">
-        <v>3.1821419999999998</v>
-      </c>
-      <c r="I15" s="56">
-        <v>2.4300489999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="56">
-        <v>2.5817999999999999</v>
-      </c>
-      <c r="D16" s="30">
-        <v>143</v>
-      </c>
-      <c r="E16" s="30">
-        <v>587</v>
-      </c>
-      <c r="F16" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="56">
-        <v>2.012823</v>
-      </c>
-      <c r="H16" s="56">
-        <v>3.38089</v>
-      </c>
-      <c r="I16" s="56">
-        <v>2.581823</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="56">
-        <v>2.8039000000000001</v>
-      </c>
-      <c r="D17" s="30">
-        <v>143</v>
-      </c>
-      <c r="E17" s="30">
-        <v>587</v>
-      </c>
-      <c r="F17" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="56">
-        <v>2.185988</v>
-      </c>
-      <c r="H17" s="56">
-        <v>3.6717</v>
-      </c>
-      <c r="I17" s="56">
-        <v>2.8039399999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="56">
-        <v>2.5817000000000001</v>
-      </c>
-      <c r="D18" s="30">
-        <v>143</v>
-      </c>
-      <c r="E18" s="30">
-        <v>587</v>
-      </c>
-      <c r="F18" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="56">
-        <v>2.0127030000000001</v>
-      </c>
-      <c r="H18" s="56">
-        <v>3.3806889999999998</v>
-      </c>
-      <c r="I18" s="56">
-        <v>2.5816699999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="56">
-        <v>2.6086999999999998</v>
-      </c>
-      <c r="D19" s="30">
-        <v>143</v>
-      </c>
-      <c r="E19" s="30">
-        <v>587</v>
-      </c>
-      <c r="F19" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="56">
-        <v>2.0337499999999999</v>
-      </c>
-      <c r="H19" s="56">
-        <v>3.4160520000000001</v>
-      </c>
-      <c r="I19" s="56">
-        <v>2.60867</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="30" t="s">
+      <c r="E21" s="28">
+        <v>15381</v>
+      </c>
+      <c r="F21" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="56">
-        <v>2.6669999999999998</v>
-      </c>
-      <c r="D20" s="30">
-        <v>143</v>
-      </c>
-      <c r="E20" s="30">
-        <v>587</v>
-      </c>
-      <c r="F20" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="56">
-        <v>2.0792090000000001</v>
-      </c>
-      <c r="H20" s="56">
-        <v>3.492397</v>
-      </c>
-      <c r="I20" s="56">
-        <v>2.666976</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="56">
-        <v>0.71106999999999998</v>
-      </c>
-      <c r="D21" s="30">
-        <v>2427</v>
-      </c>
-      <c r="E21" s="30">
-        <v>15381</v>
-      </c>
-      <c r="F21" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="56">
+      <c r="G21" s="54">
         <v>0.66973000000000005</v>
       </c>
-      <c r="H21" s="56">
+      <c r="H21" s="54">
         <v>0.75595999999999997</v>
       </c>
-      <c r="I21" s="56">
+      <c r="I21" s="54">
         <v>0.71106570000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
github document for analysis and qc
</commit_message>
<xml_diff>
--- a/FishLandings/output/statistics_v2.xlsx
+++ b/FishLandings/output/statistics_v2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB79DA0D-1DDA-5147-8E01-2DEDFD6A8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC902A5-752F-1C42-9DE6-61A67CF76C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="11460" windowWidth="24940" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2720" windowWidth="25740" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Per Trap Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2 Nutrients stats" sheetId="7" r:id="rId2"/>
     <sheet name="Supplemental Table 2" sheetId="8" r:id="rId3"/>
+    <sheet name="Supplemental Table 3" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t xml:space="preserve">t </t>
   </si>
@@ -627,6 +628,70 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Dependent Variable</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Generalized linear mixed model statistical output</t>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <r>
+      <t>(KES trap</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap Type </t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Trap Type * Month</t>
+  </si>
+  <si>
+    <t>Type III ANOVA Test on model: lmer(log(value) ~ trap_type*month + (1|BMU))</t>
   </si>
 </sst>
 </file>
@@ -638,7 +703,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -695,6 +760,13 @@
       <family val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -710,6 +782,21 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -735,7 +822,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -890,11 +977,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -987,9 +1123,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1055,6 +1188,69 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1373,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,24 +1587,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="2:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="J3" s="3"/>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
@@ -1447,10 +1643,10 @@
       <c r="F5" s="8">
         <v>0.60851</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="55">
         <v>262.79000000000002</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="59">
         <v>0.54339999999999999</v>
       </c>
     </row>
@@ -1468,7 +1664,7 @@
         <v>591</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="56"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
@@ -1485,23 +1681,23 @@
         <v>150</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="56"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:16" ht="18" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="39">
+      <c r="F8" s="38">
         <v>-3.2639999999999998</v>
       </c>
-      <c r="G8" s="57">
+      <c r="G8" s="56">
         <v>200.96</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="87">
         <v>1.291E-3</v>
       </c>
     </row>
@@ -1519,7 +1715,7 @@
         <v>591</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="56"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="4"/>
       <c r="J9" s="32"/>
       <c r="K9" s="3"/>
@@ -1543,7 +1739,7 @@
         <v>150</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="56"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="4"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1557,13 +1753,13 @@
       <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="39">
+      <c r="F11" s="38">
         <v>-38.104999999999997</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="56">
         <v>3592</v>
       </c>
       <c r="H11" s="29" t="s">
@@ -1591,7 +1787,7 @@
         <v>15396</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="56"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="4"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1614,7 +1810,7 @@
         <v>2428</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="56"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="4"/>
       <c r="J13" s="3"/>
       <c r="K13" s="30"/>
@@ -1628,13 +1824,13 @@
       <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="39">
+      <c r="F14" s="38">
         <v>18.172999999999998</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="56">
         <v>436.22</v>
       </c>
       <c r="H14" s="29" t="s">
@@ -1662,7 +1858,7 @@
         <v>591</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="56"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1685,7 +1881,7 @@
         <v>150</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="56"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="4"/>
       <c r="J16" s="3"/>
       <c r="K16" s="30"/>
@@ -1699,13 +1895,13 @@
       <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="39">
+      <c r="F17" s="38">
         <v>-4.8760000000000003</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="56">
         <v>202.64</v>
       </c>
       <c r="H17" s="29" t="s">
@@ -1733,7 +1929,7 @@
         <v>591</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="56"/>
+      <c r="G18" s="55"/>
       <c r="H18" s="4"/>
       <c r="J18" s="32"/>
       <c r="K18" s="3"/>
@@ -1757,7 +1953,7 @@
         <v>150</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="56"/>
+      <c r="G19" s="55"/>
       <c r="H19" s="4"/>
       <c r="J19" s="3"/>
       <c r="K19" s="30"/>
@@ -1771,16 +1967,16 @@
       <c r="B20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="39">
+      <c r="F20" s="38">
         <v>-3.0569000000000002</v>
       </c>
-      <c r="G20" s="57">
+      <c r="G20" s="56">
         <v>41.628999999999998</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="87">
         <v>3.8969999999999999E-3</v>
       </c>
       <c r="J20" s="3"/>
@@ -1805,7 +2001,7 @@
         <v>352</v>
       </c>
       <c r="F21" s="8"/>
-      <c r="G21" s="56"/>
+      <c r="G21" s="55"/>
       <c r="H21" s="4"/>
       <c r="J21" s="32"/>
       <c r="K21" s="3"/>
@@ -1829,7 +2025,7 @@
         <v>40</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="56"/>
+      <c r="G22" s="55"/>
       <c r="H22" s="4"/>
       <c r="J22" s="3"/>
       <c r="K22" s="30"/>
@@ -1843,13 +2039,13 @@
       <c r="B23" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="39">
+      <c r="F23" s="38">
         <v>-2.9051</v>
       </c>
-      <c r="G23" s="57">
+      <c r="G23" s="56">
         <v>206.42</v>
       </c>
       <c r="H23" s="29">
@@ -1877,7 +2073,7 @@
         <v>590</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="56"/>
+      <c r="G24" s="55"/>
       <c r="H24" s="4"/>
       <c r="J24" s="32"/>
       <c r="K24" s="3"/>
@@ -1901,7 +2097,7 @@
         <v>147</v>
       </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="58"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="5"/>
       <c r="J25" s="3"/>
       <c r="K25" s="30"/>
@@ -1915,16 +2111,16 @@
       <c r="B26" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="39">
+      <c r="F26" s="38">
         <v>-1.7276</v>
       </c>
-      <c r="G26" s="57">
+      <c r="G26" s="56">
         <v>27.716999999999999</v>
       </c>
-      <c r="H26" s="63">
+      <c r="H26" s="62">
         <v>9.5189999999999997E-2</v>
       </c>
       <c r="J26" s="3"/>
@@ -1949,7 +2145,7 @@
         <v>93</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="56"/>
+      <c r="G27" s="55"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
@@ -1966,20 +2162,20 @@
         <v>17</v>
       </c>
       <c r="F28" s="10"/>
-      <c r="G28" s="58"/>
+      <c r="G28" s="57"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="39">
+      <c r="F29" s="38">
         <v>-20.591999999999999</v>
       </c>
-      <c r="G29" s="57">
+      <c r="G29" s="56">
         <v>3596.2</v>
       </c>
       <c r="H29" s="29" t="s">
@@ -2000,7 +2196,7 @@
         <v>15382</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="56"/>
+      <c r="G30" s="55"/>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
@@ -2017,7 +2213,7 @@
         <v>2428</v>
       </c>
       <c r="F31" s="10"/>
-      <c r="G31" s="58"/>
+      <c r="G31" s="57"/>
       <c r="H31" s="5"/>
     </row>
   </sheetData>
@@ -2032,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE17491E-AE3E-0847-8740-D1EE4E6F1D7A}">
   <dimension ref="B4:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2045,24 +2241,24 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
     </row>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
@@ -2100,7 +2296,7 @@
       <c r="G7" s="21">
         <v>735</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="58">
         <v>4.7739999999999996E-3</v>
       </c>
     </row>
@@ -2119,7 +2315,7 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="60"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
@@ -2136,7 +2332,7 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="60"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
@@ -2151,7 +2347,7 @@
       <c r="G10" s="24">
         <v>204.14</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="60">
         <v>5.3019999999999999E-4</v>
       </c>
     </row>
@@ -2170,7 +2366,7 @@
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="60"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
@@ -2187,7 +2383,7 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="60"/>
+      <c r="H12" s="59"/>
     </row>
     <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
@@ -2202,7 +2398,7 @@
       <c r="G13" s="24">
         <v>200.86</v>
       </c>
-      <c r="H13" s="61" t="s">
+      <c r="H13" s="60" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2221,7 +2417,7 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="60"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
@@ -2238,7 +2434,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="60"/>
+      <c r="H15" s="59"/>
     </row>
     <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B16" s="37" t="s">
@@ -2272,7 +2468,7 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="60"/>
+      <c r="H17" s="59"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="36" t="s">
@@ -2289,7 +2485,7 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="60"/>
+      <c r="H18" s="59"/>
     </row>
     <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
@@ -2304,7 +2500,7 @@
       <c r="G19" s="24">
         <v>735</v>
       </c>
-      <c r="H19" s="61">
+      <c r="H19" s="60">
         <v>2.9770000000000001E-2</v>
       </c>
     </row>
@@ -2323,13 +2519,13 @@
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="60"/>
+      <c r="H20" s="59"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="54">
         <v>381.39269999999999</v>
       </c>
       <c r="D21" s="27">
@@ -2340,7 +2536,7 @@
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="62"/>
+      <c r="H21" s="61"/>
     </row>
     <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
@@ -2355,7 +2551,7 @@
       <c r="G22" s="24">
         <v>204.27</v>
       </c>
-      <c r="H22" s="61">
+      <c r="H22" s="60">
         <v>1.687E-2</v>
       </c>
     </row>
@@ -2374,13 +2570,13 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="60"/>
+      <c r="H23" s="59"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="54">
         <v>21.090299999999999</v>
       </c>
       <c r="D24" s="27">
@@ -2391,7 +2587,7 @@
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="62"/>
+      <c r="H24" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2405,8 +2601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9E1C08-A7E9-C84F-8ABE-E7EF96EBA4D4}">
   <dimension ref="B3:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2424,62 +2620,62 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" ht="19" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="52"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="42" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2487,25 +2683,25 @@
       <c r="B7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="46">
         <v>0.72887999999999997</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="47">
         <v>149</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="47">
         <v>590</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="49">
         <v>1.9599999999999999E-2</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="46">
         <v>0.57044059999999996</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="46">
         <v>0.94976649999999996</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="46">
         <v>0.72887690000000005</v>
       </c>
     </row>
@@ -2513,25 +2709,25 @@
       <c r="B8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="46">
         <v>1.5349999999999999</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="47">
         <v>149</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="47">
         <v>590</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="49">
         <v>5.2970000000000003E-4</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="46">
         <v>1.201322</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="46">
         <v>2.0001639999999998</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="46">
         <v>1.5349809999999999</v>
       </c>
     </row>
@@ -2539,7 +2735,7 @@
       <c r="B9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="53">
         <v>0.71281000000000005</v>
       </c>
       <c r="D9" s="28">
@@ -2548,16 +2744,16 @@
       <c r="E9" s="28">
         <v>15395</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="53">
         <v>0.67137999999999998</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="53">
         <v>0.7578146</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="53">
         <v>0.7128101</v>
       </c>
     </row>
@@ -2565,7 +2761,7 @@
       <c r="B10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="53">
         <v>0.29304999999999998</v>
       </c>
       <c r="D10" s="28">
@@ -2574,16 +2770,16 @@
       <c r="E10" s="28">
         <v>590</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="53">
         <v>0.22935</v>
       </c>
-      <c r="H10" s="54">
+      <c r="H10" s="53">
         <v>0.3818608</v>
       </c>
-      <c r="I10" s="54">
+      <c r="I10" s="53">
         <v>0.29305049999999999</v>
       </c>
     </row>
@@ -2591,7 +2787,7 @@
       <c r="B11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="53">
         <v>1.4890000000000001</v>
       </c>
       <c r="D11" s="28">
@@ -2600,16 +2796,16 @@
       <c r="E11" s="28">
         <v>590</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="52">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="53">
         <v>1.1653009999999999</v>
       </c>
-      <c r="H11" s="54">
+      <c r="H11" s="53">
         <v>1.9401919999999999</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="53">
         <v>1.4889570000000001</v>
       </c>
     </row>
@@ -2617,7 +2813,7 @@
       <c r="B12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="53">
         <v>3.4214000000000002</v>
       </c>
       <c r="D12" s="28">
@@ -2626,16 +2822,16 @@
       <c r="E12" s="28">
         <v>351</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="53">
         <v>2.2290230000000002</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="53">
         <v>5.7458809999999998</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I12" s="53">
         <v>3.4213550000000001</v>
       </c>
     </row>
@@ -2643,7 +2839,7 @@
       <c r="B13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="53">
         <v>1.2803</v>
       </c>
       <c r="D13" s="28">
@@ -2652,16 +2848,16 @@
       <c r="E13" s="28">
         <v>589</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="49">
         <v>4.9910000000000003E-2</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="53">
         <v>1</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="53">
         <v>1.6722729999999999</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="53">
         <v>1.2802640000000001</v>
       </c>
     </row>
@@ -2669,7 +2865,7 @@
       <c r="B14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="53">
         <v>0.55650999999999995</v>
       </c>
       <c r="D14" s="28">
@@ -2681,13 +2877,13 @@
       <c r="F14" s="28">
         <v>0.1842</v>
       </c>
-      <c r="G14" s="54">
+      <c r="G14" s="53">
         <v>0.28520699999999999</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H14" s="53">
         <v>1.3372200000000001</v>
       </c>
-      <c r="I14" s="54">
+      <c r="I14" s="53">
         <v>0.55651170000000005</v>
       </c>
     </row>
@@ -2695,7 +2891,7 @@
       <c r="B15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="53">
         <v>1.2085999999999999</v>
       </c>
       <c r="D15" s="28">
@@ -2704,16 +2900,16 @@
       <c r="E15" s="28">
         <v>589</v>
       </c>
-      <c r="F15" s="49">
+      <c r="F15" s="48">
         <v>0.13320000000000001</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="53">
         <v>0.94410550000000004</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="53">
         <v>1.5786553999999999</v>
       </c>
-      <c r="I15" s="54">
+      <c r="I15" s="53">
         <v>1.2085920000000001</v>
       </c>
     </row>
@@ -2721,7 +2917,7 @@
       <c r="B16" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="53">
         <v>1.3280000000000001</v>
       </c>
       <c r="D16" s="28">
@@ -2730,16 +2926,16 @@
       <c r="E16" s="28">
         <v>589</v>
       </c>
-      <c r="F16" s="50">
+      <c r="F16" s="49">
         <v>2.4129999999999999E-2</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="53">
         <v>1.0373000000000001</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="53">
         <v>1.7345999999999999</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="53">
         <v>1.3279810000000001</v>
       </c>
     </row>
@@ -2747,7 +2943,7 @@
       <c r="B17" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="53">
         <v>1.4037999999999999</v>
       </c>
       <c r="D17" s="28">
@@ -2756,16 +2952,16 @@
       <c r="E17" s="28">
         <v>589</v>
       </c>
-      <c r="F17" s="50">
+      <c r="F17" s="49">
         <v>6.829E-3</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="53">
         <v>1.0965800000000001</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="53">
         <v>1.8335999999999999</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I17" s="53">
         <v>1.40378</v>
       </c>
     </row>
@@ -2773,7 +2969,7 @@
       <c r="B18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="53">
         <v>1.1881999999999999</v>
       </c>
       <c r="D18" s="28">
@@ -2782,24 +2978,24 @@
       <c r="E18" s="28">
         <v>589</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="47">
         <v>0.17169999999999999</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="53">
         <v>0.928176</v>
       </c>
-      <c r="H18" s="54">
+      <c r="H18" s="53">
         <v>1.552019</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="53">
         <v>1.188199</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="53">
         <v>0.96296999999999999</v>
       </c>
       <c r="D19" s="28">
@@ -2808,16 +3004,16 @@
       <c r="E19" s="28">
         <v>589</v>
       </c>
-      <c r="F19" s="48">
+      <c r="F19" s="47">
         <v>0.79410000000000003</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="53">
         <v>0.75223839999999997</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H19" s="53">
         <v>1.2578311</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I19" s="53">
         <v>0.962974</v>
       </c>
     </row>
@@ -2825,7 +3021,7 @@
       <c r="B20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="53">
         <v>1.3251999999999999</v>
       </c>
       <c r="D20" s="28">
@@ -2834,16 +3030,16 @@
       <c r="E20" s="28">
         <v>589</v>
       </c>
-      <c r="F20" s="53">
+      <c r="F20" s="52">
         <v>2.52E-2</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="53">
         <v>1.035229</v>
       </c>
-      <c r="H20" s="54">
+      <c r="H20" s="53">
         <v>1.731025</v>
       </c>
-      <c r="I20" s="54">
+      <c r="I20" s="53">
         <v>1.3252429999999999</v>
       </c>
     </row>
@@ -2851,7 +3047,7 @@
       <c r="B21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="53">
         <v>0.71106999999999998</v>
       </c>
       <c r="D21" s="28">
@@ -2860,16 +3056,16 @@
       <c r="E21" s="28">
         <v>15381</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="53">
         <v>0.66973000000000005</v>
       </c>
-      <c r="H21" s="54">
+      <c r="H21" s="53">
         <v>0.75595999999999997</v>
       </c>
-      <c r="I21" s="54">
+      <c r="I21" s="53">
         <v>0.71106570000000002</v>
       </c>
     </row>
@@ -2880,4 +3076,173 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8016EE-6AD0-3B41-A700-F15356CEFD52}">
+  <dimension ref="C3:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+    </row>
+    <row r="4" spans="3:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+    </row>
+    <row r="5" spans="3:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0.38169999999999998</v>
+      </c>
+      <c r="F6" s="71">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.53670300000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="C7" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="30">
+        <v>199.07900000000001</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="68"/>
+      <c r="D8" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="72">
+        <v>16.1967</v>
+      </c>
+      <c r="F8" s="73">
+        <v>5</v>
+      </c>
+      <c r="G8" s="75">
+        <v>6.3039999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="84"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="85"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="86"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="77"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="81"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C9:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>